<commit_message>
Misurati speedup e throughput per bf0-mutex su GTX 1070
</commit_message>
<xml_diff>
--- a/performance bf0.xlsx
+++ b/performance bf0.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Filippo\Desktop\tesi\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{82CF8E20-3AA0-49A2-BC41-463BE148BB7C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C48B78B9-6B8E-4322-BE23-D813F0BD29AD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -322,16 +322,16 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normale" xfId="0" builtinId="0"/>
@@ -614,8 +614,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AO83"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="G9" workbookViewId="0">
-      <selection activeCell="AI43" sqref="AI43"/>
+    <sheetView tabSelected="1" topLeftCell="G54" workbookViewId="0">
+      <selection activeCell="AI83" sqref="AI83"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -815,7 +815,7 @@
       </c>
     </row>
     <row r="5" spans="1:41" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="19" t="s">
+      <c r="A5" s="22" t="s">
         <v>10</v>
       </c>
       <c r="B5" s="4" t="s">
@@ -859,7 +859,7 @@
         <v>#DIV/0!</v>
       </c>
       <c r="U5" s="15"/>
-      <c r="V5" s="19" t="s">
+      <c r="V5" s="22" t="s">
         <v>10</v>
       </c>
       <c r="W5" s="4" t="s">
@@ -904,7 +904,7 @@
       </c>
     </row>
     <row r="6" spans="1:41" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="19"/>
+      <c r="A6" s="22"/>
       <c r="B6" s="4" t="s">
         <v>2</v>
       </c>
@@ -926,7 +926,7 @@
       <c r="K6" s="10">
         <v>0.93400000000000005</v>
       </c>
-      <c r="L6" s="22">
+      <c r="L6" s="19">
         <v>0.93</v>
       </c>
       <c r="M6" s="11">
@@ -946,7 +946,7 @@
         <v>#DIV/0!</v>
       </c>
       <c r="U6" s="15"/>
-      <c r="V6" s="19"/>
+      <c r="V6" s="22"/>
       <c r="W6" s="4" t="s">
         <v>2</v>
       </c>
@@ -968,7 +968,7 @@
       <c r="AF6" s="10">
         <v>6299</v>
       </c>
-      <c r="AG6" s="22">
+      <c r="AG6" s="19">
         <v>6323</v>
       </c>
       <c r="AH6" s="11">
@@ -989,7 +989,7 @@
       </c>
     </row>
     <row r="7" spans="1:41" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="19"/>
+      <c r="A7" s="22"/>
       <c r="B7" s="4" t="s">
         <v>3</v>
       </c>
@@ -1011,7 +1011,7 @@
       <c r="K7" s="10">
         <v>2.944</v>
       </c>
-      <c r="L7" s="22">
+      <c r="L7" s="19">
         <v>2.9550000000000001</v>
       </c>
       <c r="M7" s="11">
@@ -1031,7 +1031,7 @@
         <v>#DIV/0!</v>
       </c>
       <c r="U7" s="15"/>
-      <c r="V7" s="19"/>
+      <c r="V7" s="22"/>
       <c r="W7" s="4" t="s">
         <v>3</v>
       </c>
@@ -1053,7 +1053,7 @@
       <c r="AF7" s="10">
         <v>7088</v>
       </c>
-      <c r="AG7" s="22">
+      <c r="AG7" s="19">
         <v>7061</v>
       </c>
       <c r="AH7" s="11">
@@ -1074,7 +1074,7 @@
       </c>
     </row>
     <row r="8" spans="1:41" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="19"/>
+      <c r="A8" s="22"/>
       <c r="B8" s="4" t="s">
         <v>4</v>
       </c>
@@ -1090,13 +1090,13 @@
       <c r="I8" s="9">
         <v>8.9440000000000008</v>
       </c>
-      <c r="J8" s="22">
+      <c r="J8" s="19">
         <v>8.9</v>
       </c>
-      <c r="K8" s="22">
+      <c r="K8" s="19">
         <v>8.8979999999999997</v>
       </c>
-      <c r="L8" s="22">
+      <c r="L8" s="19">
         <v>8.9090000000000007</v>
       </c>
       <c r="M8" s="11">
@@ -1116,7 +1116,7 @@
         <v>#DIV/0!</v>
       </c>
       <c r="U8" s="15"/>
-      <c r="V8" s="19"/>
+      <c r="V8" s="22"/>
       <c r="W8" s="4" t="s">
         <v>4</v>
       </c>
@@ -1132,13 +1132,13 @@
       <c r="AD8" s="9">
         <v>9258</v>
       </c>
-      <c r="AE8" s="22">
+      <c r="AE8" s="19">
         <v>9303</v>
       </c>
-      <c r="AF8" s="22">
+      <c r="AF8" s="19">
         <v>9306</v>
       </c>
-      <c r="AG8" s="22">
+      <c r="AG8" s="19">
         <v>9294</v>
       </c>
       <c r="AH8" s="11">
@@ -1159,7 +1159,7 @@
       </c>
     </row>
     <row r="9" spans="1:41" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="19"/>
+      <c r="A9" s="22"/>
       <c r="B9" s="4" t="s">
         <v>5</v>
       </c>
@@ -1175,13 +1175,13 @@
       <c r="I9" s="9">
         <v>15.941000000000001</v>
       </c>
-      <c r="J9" s="22">
+      <c r="J9" s="19">
         <v>15.919</v>
       </c>
-      <c r="K9" s="22">
+      <c r="K9" s="19">
         <v>15.907999999999999</v>
       </c>
-      <c r="L9" s="22">
+      <c r="L9" s="19">
         <v>15.882</v>
       </c>
       <c r="M9" s="11">
@@ -1201,7 +1201,7 @@
         <v>#DIV/0!</v>
       </c>
       <c r="U9" s="15"/>
-      <c r="V9" s="19"/>
+      <c r="V9" s="22"/>
       <c r="W9" s="4" t="s">
         <v>5</v>
       </c>
@@ -1217,13 +1217,13 @@
       <c r="AD9" s="9">
         <v>10130</v>
       </c>
-      <c r="AE9" s="22">
+      <c r="AE9" s="19">
         <v>10140</v>
       </c>
-      <c r="AF9" s="22">
+      <c r="AF9" s="19">
         <v>10150</v>
       </c>
-      <c r="AG9" s="22">
+      <c r="AG9" s="19">
         <v>10160</v>
       </c>
       <c r="AH9" s="11">
@@ -1244,7 +1244,7 @@
       </c>
     </row>
     <row r="10" spans="1:41" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="19"/>
+      <c r="A10" s="22"/>
       <c r="B10" s="4" t="s">
         <v>6</v>
       </c>
@@ -1260,13 +1260,13 @@
       <c r="I10" s="9">
         <v>0.27300000000000002</v>
       </c>
-      <c r="J10" s="22">
+      <c r="J10" s="19">
         <v>0.26900000000000002</v>
       </c>
-      <c r="K10" s="22">
+      <c r="K10" s="19">
         <v>0.27500000000000002</v>
       </c>
-      <c r="L10" s="22">
+      <c r="L10" s="19">
         <v>0.28000000000000003</v>
       </c>
       <c r="M10" s="11">
@@ -1286,7 +1286,7 @@
         <v>#DIV/0!</v>
       </c>
       <c r="U10" s="15"/>
-      <c r="V10" s="19"/>
+      <c r="V10" s="22"/>
       <c r="W10" s="4" t="s">
         <v>6</v>
       </c>
@@ -1302,13 +1302,13 @@
       <c r="AD10" s="9">
         <v>915.3</v>
       </c>
-      <c r="AE10" s="22">
+      <c r="AE10" s="19">
         <v>928.5</v>
       </c>
-      <c r="AF10" s="22">
+      <c r="AF10" s="19">
         <v>908.1</v>
       </c>
-      <c r="AG10" s="22">
+      <c r="AG10" s="19">
         <v>893.2</v>
       </c>
       <c r="AH10" s="11">
@@ -1329,7 +1329,7 @@
       </c>
     </row>
     <row r="11" spans="1:41" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="19"/>
+      <c r="A11" s="22"/>
       <c r="B11" s="4" t="s">
         <v>7</v>
       </c>
@@ -1345,13 +1345,13 @@
       <c r="I11" s="9">
         <v>0.31900000000000001</v>
       </c>
-      <c r="J11" s="22">
+      <c r="J11" s="19">
         <v>0.29599999999999999</v>
       </c>
-      <c r="K11" s="22">
+      <c r="K11" s="19">
         <v>0.28199999999999997</v>
       </c>
-      <c r="L11" s="22">
+      <c r="L11" s="19">
         <v>0.28100000000000003</v>
       </c>
       <c r="M11" s="11">
@@ -1371,7 +1371,7 @@
         <v>#DIV/0!</v>
       </c>
       <c r="U11" s="15"/>
-      <c r="V11" s="19"/>
+      <c r="V11" s="22"/>
       <c r="W11" s="4" t="s">
         <v>7</v>
       </c>
@@ -1387,13 +1387,13 @@
       <c r="AD11" s="9">
         <v>1567</v>
       </c>
-      <c r="AE11" s="22">
+      <c r="AE11" s="19">
         <v>1689</v>
       </c>
-      <c r="AF11" s="22">
+      <c r="AF11" s="19">
         <v>1774</v>
       </c>
-      <c r="AG11" s="22">
+      <c r="AG11" s="19">
         <v>1777</v>
       </c>
       <c r="AH11" s="11">
@@ -1414,7 +1414,7 @@
       </c>
     </row>
     <row r="12" spans="1:41" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="19"/>
+      <c r="A12" s="22"/>
       <c r="B12" s="4" t="s">
         <v>8</v>
       </c>
@@ -1430,13 +1430,13 @@
       <c r="I12" s="9">
         <v>0.318</v>
       </c>
-      <c r="J12" s="22">
+      <c r="J12" s="19">
         <v>0.29899999999999999</v>
       </c>
-      <c r="K12" s="22">
+      <c r="K12" s="19">
         <v>0.309</v>
       </c>
-      <c r="L12" s="22">
+      <c r="L12" s="19">
         <v>0.29499999999999998</v>
       </c>
       <c r="M12" s="11">
@@ -1456,7 +1456,7 @@
         <v>#DIV/0!</v>
       </c>
       <c r="U12" s="15"/>
-      <c r="V12" s="19"/>
+      <c r="V12" s="22"/>
       <c r="W12" s="4" t="s">
         <v>8</v>
       </c>
@@ -1472,13 +1472,13 @@
       <c r="AD12" s="9">
         <v>2357</v>
       </c>
-      <c r="AE12" s="22">
+      <c r="AE12" s="19">
         <v>2504</v>
       </c>
-      <c r="AF12" s="22">
+      <c r="AF12" s="19">
         <v>2427</v>
       </c>
-      <c r="AG12" s="22">
+      <c r="AG12" s="19">
         <v>2544</v>
       </c>
       <c r="AH12" s="11">
@@ -1499,7 +1499,7 @@
       </c>
     </row>
     <row r="13" spans="1:41" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="19"/>
+      <c r="A13" s="22"/>
       <c r="B13" s="4" t="s">
         <v>9</v>
       </c>
@@ -1541,7 +1541,7 @@
         <v>#DIV/0!</v>
       </c>
       <c r="U13" s="15"/>
-      <c r="V13" s="19"/>
+      <c r="V13" s="22"/>
       <c r="W13" s="4" t="s">
         <v>9</v>
       </c>
@@ -1627,7 +1627,7 @@
       <c r="AO14" s="15"/>
     </row>
     <row r="15" spans="1:41" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="19" t="s">
+      <c r="A15" s="22" t="s">
         <v>20</v>
       </c>
       <c r="B15" s="4" t="s">
@@ -1671,7 +1671,7 @@
         <v>#DIV/0!</v>
       </c>
       <c r="U15" s="15"/>
-      <c r="V15" s="19" t="s">
+      <c r="V15" s="22" t="s">
         <v>20</v>
       </c>
       <c r="W15" s="4" t="s">
@@ -1716,7 +1716,7 @@
       </c>
     </row>
     <row r="16" spans="1:41" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="19"/>
+      <c r="A16" s="22"/>
       <c r="B16" s="4" t="s">
         <v>2</v>
       </c>
@@ -1732,13 +1732,13 @@
       <c r="I16" s="9">
         <v>1.056</v>
       </c>
-      <c r="J16" s="22">
+      <c r="J16" s="19">
         <v>0.94199999999999995</v>
       </c>
-      <c r="K16" s="22">
+      <c r="K16" s="19">
         <v>0.98199999999999998</v>
       </c>
-      <c r="L16" s="22">
+      <c r="L16" s="19">
         <v>0.99399999999999999</v>
       </c>
       <c r="M16" s="11">
@@ -1758,7 +1758,7 @@
         <v>#DIV/0!</v>
       </c>
       <c r="U16" s="15"/>
-      <c r="V16" s="19"/>
+      <c r="V16" s="22"/>
       <c r="W16" s="4" t="s">
         <v>2</v>
       </c>
@@ -1774,13 +1774,13 @@
       <c r="AD16" s="9">
         <v>5566</v>
       </c>
-      <c r="AE16" s="22">
+      <c r="AE16" s="19">
         <v>6240</v>
       </c>
-      <c r="AF16" s="22">
+      <c r="AF16" s="19">
         <v>5990</v>
       </c>
-      <c r="AG16" s="22">
+      <c r="AG16" s="19">
         <v>5914</v>
       </c>
       <c r="AH16" s="11">
@@ -1801,7 +1801,7 @@
       </c>
     </row>
     <row r="17" spans="1:41" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="19"/>
+      <c r="A17" s="22"/>
       <c r="B17" s="4" t="s">
         <v>3</v>
       </c>
@@ -1817,13 +1817,13 @@
       <c r="I17" s="9">
         <v>2.879</v>
       </c>
-      <c r="J17" s="22">
+      <c r="J17" s="19">
         <v>2.843</v>
       </c>
-      <c r="K17" s="22">
+      <c r="K17" s="19">
         <v>2.7959999999999998</v>
       </c>
-      <c r="L17" s="22">
+      <c r="L17" s="19">
         <v>2.8029999999999999</v>
       </c>
       <c r="M17" s="11">
@@ -1843,7 +1843,7 @@
         <v>#DIV/0!</v>
       </c>
       <c r="U17" s="15"/>
-      <c r="V17" s="19"/>
+      <c r="V17" s="22"/>
       <c r="W17" s="4" t="s">
         <v>3</v>
       </c>
@@ -1859,13 +1859,13 @@
       <c r="AD17" s="9">
         <v>7247</v>
       </c>
-      <c r="AE17" s="22">
+      <c r="AE17" s="19">
         <v>7340</v>
       </c>
-      <c r="AF17" s="22">
+      <c r="AF17" s="19">
         <v>7463</v>
       </c>
-      <c r="AG17" s="22">
+      <c r="AG17" s="19">
         <v>7445</v>
       </c>
       <c r="AH17" s="11">
@@ -1886,7 +1886,7 @@
       </c>
     </row>
     <row r="18" spans="1:41" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="19"/>
+      <c r="A18" s="22"/>
       <c r="B18" s="4" t="s">
         <v>4</v>
       </c>
@@ -1902,13 +1902,13 @@
       <c r="I18" s="9">
         <v>8.6059999999999999</v>
       </c>
-      <c r="J18" s="22">
+      <c r="J18" s="19">
         <v>8.3800000000000008</v>
       </c>
-      <c r="K18" s="22">
+      <c r="K18" s="19">
         <v>8.5649999999999995</v>
       </c>
-      <c r="L18" s="22">
+      <c r="L18" s="19">
         <v>8.4870000000000001</v>
       </c>
       <c r="M18" s="11">
@@ -1928,7 +1928,7 @@
         <v>#DIV/0!</v>
       </c>
       <c r="U18" s="15"/>
-      <c r="V18" s="19"/>
+      <c r="V18" s="22"/>
       <c r="W18" s="4" t="s">
         <v>4</v>
       </c>
@@ -1944,13 +1944,13 @@
       <c r="AD18" s="9">
         <v>9622</v>
       </c>
-      <c r="AE18" s="22">
+      <c r="AE18" s="19">
         <v>9881</v>
       </c>
-      <c r="AF18" s="22">
+      <c r="AF18" s="19">
         <v>9667</v>
       </c>
-      <c r="AG18" s="22">
+      <c r="AG18" s="19">
         <v>9757</v>
       </c>
       <c r="AH18" s="11">
@@ -1971,7 +1971,7 @@
       </c>
     </row>
     <row r="19" spans="1:41" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="19"/>
+      <c r="A19" s="22"/>
       <c r="B19" s="4" t="s">
         <v>5</v>
       </c>
@@ -1987,13 +1987,13 @@
       <c r="I19" s="9">
         <v>15.096</v>
       </c>
-      <c r="J19" s="22">
+      <c r="J19" s="19">
         <v>14.930999999999999</v>
       </c>
-      <c r="K19" s="22">
+      <c r="K19" s="19">
         <v>14.848000000000001</v>
       </c>
-      <c r="L19" s="22">
+      <c r="L19" s="19">
         <v>15.087</v>
       </c>
       <c r="M19" s="11">
@@ -2013,7 +2013,7 @@
         <v>#DIV/0!</v>
       </c>
       <c r="U19" s="15"/>
-      <c r="V19" s="19"/>
+      <c r="V19" s="22"/>
       <c r="W19" s="4" t="s">
         <v>5</v>
       </c>
@@ -2029,13 +2029,13 @@
       <c r="AD19" s="9">
         <v>10690</v>
       </c>
-      <c r="AE19" s="22">
+      <c r="AE19" s="19">
         <v>10810</v>
       </c>
-      <c r="AF19" s="22">
+      <c r="AF19" s="19">
         <v>10870</v>
       </c>
-      <c r="AG19" s="22">
+      <c r="AG19" s="19">
         <v>10700</v>
       </c>
       <c r="AH19" s="11">
@@ -2056,7 +2056,7 @@
       </c>
     </row>
     <row r="20" spans="1:41" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="19"/>
+      <c r="A20" s="22"/>
       <c r="B20" s="4" t="s">
         <v>6</v>
       </c>
@@ -2072,13 +2072,13 @@
       <c r="I20" s="9">
         <v>0.29199999999999998</v>
       </c>
-      <c r="J20" s="22">
+      <c r="J20" s="19">
         <v>0.28100000000000003</v>
       </c>
-      <c r="K20" s="22">
+      <c r="K20" s="19">
         <v>0.26</v>
       </c>
-      <c r="L20" s="22">
+      <c r="L20" s="19">
         <v>0.28100000000000003</v>
       </c>
       <c r="M20" s="11">
@@ -2098,7 +2098,7 @@
         <v>#DIV/0!</v>
       </c>
       <c r="U20" s="15"/>
-      <c r="V20" s="19"/>
+      <c r="V20" s="22"/>
       <c r="W20" s="4" t="s">
         <v>6</v>
       </c>
@@ -2114,13 +2114,13 @@
       <c r="AD20" s="9">
         <v>854.7</v>
       </c>
-      <c r="AE20" s="22">
+      <c r="AE20" s="19">
         <v>889.2</v>
       </c>
-      <c r="AF20" s="22">
+      <c r="AF20" s="19">
         <v>961.3</v>
       </c>
-      <c r="AG20" s="22">
+      <c r="AG20" s="19">
         <v>889.7</v>
       </c>
       <c r="AH20" s="11">
@@ -2141,7 +2141,7 @@
       </c>
     </row>
     <row r="21" spans="1:41" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="19"/>
+      <c r="A21" s="22"/>
       <c r="B21" s="4" t="s">
         <v>7</v>
       </c>
@@ -2157,13 +2157,13 @@
       <c r="I21" s="9">
         <v>0.309</v>
       </c>
-      <c r="J21" s="22">
+      <c r="J21" s="19">
         <v>0.30299999999999999</v>
       </c>
-      <c r="K21" s="22">
+      <c r="K21" s="19">
         <v>0.26800000000000002</v>
       </c>
-      <c r="L21" s="22">
+      <c r="L21" s="19">
         <v>0.27600000000000002</v>
       </c>
       <c r="M21" s="11">
@@ -2183,7 +2183,7 @@
         <v>#DIV/0!</v>
       </c>
       <c r="U21" s="15"/>
-      <c r="V21" s="19"/>
+      <c r="V21" s="22"/>
       <c r="W21" s="4" t="s">
         <v>7</v>
       </c>
@@ -2199,13 +2199,13 @@
       <c r="AD21" s="9">
         <v>1614</v>
       </c>
-      <c r="AE21" s="22">
+      <c r="AE21" s="19">
         <v>1651</v>
       </c>
-      <c r="AF21" s="22">
+      <c r="AF21" s="19">
         <v>1861</v>
       </c>
-      <c r="AG21" s="22">
+      <c r="AG21" s="19">
         <v>1809</v>
       </c>
       <c r="AH21" s="11">
@@ -2226,7 +2226,7 @@
       </c>
     </row>
     <row r="22" spans="1:41" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="19"/>
+      <c r="A22" s="22"/>
       <c r="B22" s="4" t="s">
         <v>8</v>
       </c>
@@ -2242,13 +2242,13 @@
       <c r="I22" s="9">
         <v>0.33300000000000002</v>
       </c>
-      <c r="J22" s="22">
+      <c r="J22" s="19">
         <v>0.307</v>
       </c>
-      <c r="K22" s="22">
+      <c r="K22" s="19">
         <v>0.27200000000000002</v>
       </c>
-      <c r="L22" s="22">
+      <c r="L22" s="19">
         <v>0.30099999999999999</v>
       </c>
       <c r="M22" s="11">
@@ -2268,7 +2268,7 @@
         <v>#DIV/0!</v>
       </c>
       <c r="U22" s="15"/>
-      <c r="V22" s="19"/>
+      <c r="V22" s="22"/>
       <c r="W22" s="4" t="s">
         <v>8</v>
       </c>
@@ -2284,13 +2284,13 @@
       <c r="AD22" s="9">
         <v>2250</v>
       </c>
-      <c r="AE22" s="22">
+      <c r="AE22" s="19">
         <v>2441</v>
       </c>
-      <c r="AF22" s="22">
+      <c r="AF22" s="19">
         <v>2756</v>
       </c>
-      <c r="AG22" s="22">
+      <c r="AG22" s="19">
         <v>2488</v>
       </c>
       <c r="AH22" s="11">
@@ -2311,7 +2311,7 @@
       </c>
     </row>
     <row r="23" spans="1:41" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A23" s="19"/>
+      <c r="A23" s="22"/>
       <c r="B23" s="4" t="s">
         <v>9</v>
       </c>
@@ -2353,7 +2353,7 @@
         <v>#DIV/0!</v>
       </c>
       <c r="U23" s="15"/>
-      <c r="V23" s="19"/>
+      <c r="V23" s="22"/>
       <c r="W23" s="4" t="s">
         <v>9</v>
       </c>
@@ -2439,7 +2439,7 @@
       <c r="AO24" s="15"/>
     </row>
     <row r="25" spans="1:41" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A25" s="19" t="s">
+      <c r="A25" s="22" t="s">
         <v>21</v>
       </c>
       <c r="B25" s="4" t="s">
@@ -2483,7 +2483,7 @@
         <v>#DIV/0!</v>
       </c>
       <c r="U25" s="15"/>
-      <c r="V25" s="19" t="s">
+      <c r="V25" s="22" t="s">
         <v>21</v>
       </c>
       <c r="W25" s="4" t="s">
@@ -2528,7 +2528,7 @@
       </c>
     </row>
     <row r="26" spans="1:41" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A26" s="19"/>
+      <c r="A26" s="22"/>
       <c r="B26" s="4" t="s">
         <v>2</v>
       </c>
@@ -2544,13 +2544,13 @@
       <c r="I26" s="9">
         <v>0.96799999999999997</v>
       </c>
-      <c r="J26" s="22">
+      <c r="J26" s="19">
         <v>0.90400000000000003</v>
       </c>
-      <c r="K26" s="22">
+      <c r="K26" s="19">
         <v>0.89700000000000002</v>
       </c>
-      <c r="L26" s="22">
+      <c r="L26" s="19">
         <v>0.88600000000000001</v>
       </c>
       <c r="M26" s="11">
@@ -2570,7 +2570,7 @@
         <v>#DIV/0!</v>
       </c>
       <c r="U26" s="15"/>
-      <c r="V26" s="19"/>
+      <c r="V26" s="22"/>
       <c r="W26" s="4" t="s">
         <v>2</v>
       </c>
@@ -2586,13 +2586,13 @@
       <c r="AD26" s="9">
         <v>6077</v>
       </c>
-      <c r="AE26" s="22">
+      <c r="AE26" s="19">
         <v>6508</v>
       </c>
-      <c r="AF26" s="22">
+      <c r="AF26" s="19">
         <v>6559</v>
       </c>
-      <c r="AG26" s="22">
+      <c r="AG26" s="19">
         <v>6636</v>
       </c>
       <c r="AH26" s="11">
@@ -2613,7 +2613,7 @@
       </c>
     </row>
     <row r="27" spans="1:41" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A27" s="19"/>
+      <c r="A27" s="22"/>
       <c r="B27" s="4" t="s">
         <v>3</v>
       </c>
@@ -2629,13 +2629,13 @@
       <c r="I27" s="9">
         <v>2.7250000000000001</v>
       </c>
-      <c r="J27" s="22">
+      <c r="J27" s="19">
         <v>2.7269999999999999</v>
       </c>
-      <c r="K27" s="22">
+      <c r="K27" s="19">
         <v>2.722</v>
       </c>
-      <c r="L27" s="22">
+      <c r="L27" s="19">
         <v>2.6749999999999998</v>
       </c>
       <c r="M27" s="11">
@@ -2655,7 +2655,7 @@
         <v>#DIV/0!</v>
       </c>
       <c r="U27" s="15"/>
-      <c r="V27" s="19"/>
+      <c r="V27" s="22"/>
       <c r="W27" s="4" t="s">
         <v>3</v>
       </c>
@@ -2671,13 +2671,13 @@
       <c r="AD27" s="9">
         <v>7658</v>
       </c>
-      <c r="AE27" s="22">
+      <c r="AE27" s="19">
         <v>7652</v>
       </c>
-      <c r="AF27" s="22">
+      <c r="AF27" s="19">
         <v>7665</v>
       </c>
-      <c r="AG27" s="22">
+      <c r="AG27" s="19">
         <v>7800</v>
       </c>
       <c r="AH27" s="11">
@@ -2698,7 +2698,7 @@
       </c>
     </row>
     <row r="28" spans="1:41" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A28" s="19"/>
+      <c r="A28" s="22"/>
       <c r="B28" s="4" t="s">
         <v>4</v>
       </c>
@@ -2714,13 +2714,13 @@
       <c r="I28" s="9">
         <v>7.99</v>
       </c>
-      <c r="J28" s="22">
+      <c r="J28" s="19">
         <v>8.0440000000000005</v>
       </c>
-      <c r="K28" s="22">
+      <c r="K28" s="19">
         <v>8.0039999999999996</v>
       </c>
-      <c r="L28" s="22">
+      <c r="L28" s="19">
         <v>7.976</v>
       </c>
       <c r="M28" s="11">
@@ -2740,7 +2740,7 @@
         <v>#DIV/0!</v>
       </c>
       <c r="U28" s="15"/>
-      <c r="V28" s="19"/>
+      <c r="V28" s="22"/>
       <c r="W28" s="4" t="s">
         <v>4</v>
       </c>
@@ -2756,13 +2756,13 @@
       <c r="AD28" s="9">
         <v>10360</v>
       </c>
-      <c r="AE28" s="22">
+      <c r="AE28" s="19">
         <v>10290</v>
       </c>
-      <c r="AF28" s="22">
+      <c r="AF28" s="19">
         <v>10340</v>
       </c>
-      <c r="AG28" s="22">
+      <c r="AG28" s="19">
         <v>10380</v>
       </c>
       <c r="AH28" s="11">
@@ -2783,7 +2783,7 @@
       </c>
     </row>
     <row r="29" spans="1:41" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A29" s="19"/>
+      <c r="A29" s="22"/>
       <c r="B29" s="4" t="s">
         <v>5</v>
       </c>
@@ -2799,13 +2799,13 @@
       <c r="I29" s="9">
         <v>13.497999999999999</v>
       </c>
-      <c r="J29" s="22">
+      <c r="J29" s="19">
         <v>13.603</v>
       </c>
-      <c r="K29" s="22">
+      <c r="K29" s="19">
         <v>13.573</v>
       </c>
-      <c r="L29" s="22">
+      <c r="L29" s="19">
         <v>13.672000000000001</v>
       </c>
       <c r="M29" s="11">
@@ -2825,7 +2825,7 @@
         <v>#DIV/0!</v>
       </c>
       <c r="U29" s="15"/>
-      <c r="V29" s="19"/>
+      <c r="V29" s="22"/>
       <c r="W29" s="4" t="s">
         <v>5</v>
       </c>
@@ -2841,13 +2841,13 @@
       <c r="AD29" s="9">
         <v>11960</v>
       </c>
-      <c r="AE29" s="22">
+      <c r="AE29" s="19">
         <v>11870</v>
       </c>
-      <c r="AF29" s="22">
+      <c r="AF29" s="19">
         <v>11890</v>
       </c>
-      <c r="AG29" s="22">
+      <c r="AG29" s="19">
         <v>11810</v>
       </c>
       <c r="AH29" s="11">
@@ -2868,7 +2868,7 @@
       </c>
     </row>
     <row r="30" spans="1:41" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A30" s="19"/>
+      <c r="A30" s="22"/>
       <c r="B30" s="4" t="s">
         <v>6</v>
       </c>
@@ -2884,13 +2884,13 @@
       <c r="I30" s="9">
         <v>0.29899999999999999</v>
       </c>
-      <c r="J30" s="22">
+      <c r="J30" s="19">
         <v>0.26200000000000001</v>
       </c>
-      <c r="K30" s="22">
+      <c r="K30" s="19">
         <v>0.27700000000000002</v>
       </c>
-      <c r="L30" s="22">
+      <c r="L30" s="19">
         <v>0.27</v>
       </c>
       <c r="M30" s="11">
@@ -2910,7 +2910,7 @@
         <v>#DIV/0!</v>
       </c>
       <c r="U30" s="15"/>
-      <c r="V30" s="19"/>
+      <c r="V30" s="22"/>
       <c r="W30" s="4" t="s">
         <v>6</v>
       </c>
@@ -2926,13 +2926,13 @@
       <c r="AD30" s="9">
         <v>834.7</v>
       </c>
-      <c r="AE30" s="22">
+      <c r="AE30" s="19">
         <v>953.7</v>
       </c>
-      <c r="AF30" s="22">
+      <c r="AF30" s="19">
         <v>901.1</v>
       </c>
-      <c r="AG30" s="22">
+      <c r="AG30" s="19">
         <v>925.3</v>
       </c>
       <c r="AH30" s="11">
@@ -2953,7 +2953,7 @@
       </c>
     </row>
     <row r="31" spans="1:41" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A31" s="19"/>
+      <c r="A31" s="22"/>
       <c r="B31" s="4" t="s">
         <v>7</v>
       </c>
@@ -2969,13 +2969,13 @@
       <c r="I31" s="9">
         <v>0.312</v>
       </c>
-      <c r="J31" s="22">
+      <c r="J31" s="19">
         <v>0.28999999999999998</v>
       </c>
-      <c r="K31" s="22">
+      <c r="K31" s="19">
         <v>0.29599999999999999</v>
       </c>
-      <c r="L31" s="22">
+      <c r="L31" s="19">
         <v>0.29199999999999998</v>
       </c>
       <c r="M31" s="11">
@@ -2995,7 +2995,7 @@
         <v>#DIV/0!</v>
       </c>
       <c r="U31" s="15"/>
-      <c r="V31" s="19"/>
+      <c r="V31" s="22"/>
       <c r="W31" s="4" t="s">
         <v>7</v>
       </c>
@@ -3011,13 +3011,13 @@
       <c r="AD31" s="9">
         <v>1603</v>
       </c>
-      <c r="AE31" s="22">
+      <c r="AE31" s="19">
         <v>1725</v>
       </c>
-      <c r="AF31" s="22">
+      <c r="AF31" s="19">
         <v>1687</v>
       </c>
-      <c r="AG31" s="22">
+      <c r="AG31" s="19">
         <v>1708</v>
       </c>
       <c r="AH31" s="11">
@@ -3038,7 +3038,7 @@
       </c>
     </row>
     <row r="32" spans="1:41" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A32" s="19"/>
+      <c r="A32" s="22"/>
       <c r="B32" s="4" t="s">
         <v>8</v>
       </c>
@@ -3054,13 +3054,13 @@
       <c r="I32" s="9">
         <v>0.32900000000000001</v>
       </c>
-      <c r="J32" s="22">
+      <c r="J32" s="19">
         <v>0.30499999999999999</v>
       </c>
-      <c r="K32" s="22">
+      <c r="K32" s="19">
         <v>0.307</v>
       </c>
-      <c r="L32" s="22">
+      <c r="L32" s="19">
         <v>0.307</v>
       </c>
       <c r="M32" s="11">
@@ -3080,7 +3080,7 @@
         <v>#DIV/0!</v>
       </c>
       <c r="U32" s="15"/>
-      <c r="V32" s="19"/>
+      <c r="V32" s="22"/>
       <c r="W32" s="4" t="s">
         <v>8</v>
       </c>
@@ -3096,13 +3096,13 @@
       <c r="AD32" s="9">
         <v>2274</v>
       </c>
-      <c r="AE32" s="22">
+      <c r="AE32" s="19">
         <v>2457</v>
       </c>
-      <c r="AF32" s="22">
+      <c r="AF32" s="19">
         <v>2437</v>
       </c>
-      <c r="AG32" s="22">
+      <c r="AG32" s="19">
         <v>2442</v>
       </c>
       <c r="AH32" s="11">
@@ -3123,7 +3123,7 @@
       </c>
     </row>
     <row r="33" spans="1:41" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A33" s="19"/>
+      <c r="A33" s="22"/>
       <c r="B33" s="4" t="s">
         <v>9</v>
       </c>
@@ -3165,7 +3165,7 @@
         <v>#DIV/0!</v>
       </c>
       <c r="U33" s="15"/>
-      <c r="V33" s="19"/>
+      <c r="V33" s="22"/>
       <c r="W33" s="4" t="s">
         <v>9</v>
       </c>
@@ -3251,7 +3251,7 @@
       <c r="AO34" s="15"/>
     </row>
     <row r="35" spans="1:41" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A35" s="19" t="s">
+      <c r="A35" s="22" t="s">
         <v>22</v>
       </c>
       <c r="B35" s="4" t="s">
@@ -3295,7 +3295,7 @@
         <v>#DIV/0!</v>
       </c>
       <c r="U35" s="15"/>
-      <c r="V35" s="19" t="s">
+      <c r="V35" s="22" t="s">
         <v>22</v>
       </c>
       <c r="W35" s="4" t="s">
@@ -3340,7 +3340,7 @@
       </c>
     </row>
     <row r="36" spans="1:41" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A36" s="19"/>
+      <c r="A36" s="22"/>
       <c r="B36" s="4" t="s">
         <v>2</v>
       </c>
@@ -3356,13 +3356,13 @@
       <c r="I36" s="9">
         <v>0.99299999999999999</v>
       </c>
-      <c r="J36" s="22">
+      <c r="J36" s="19">
         <v>0.93200000000000005</v>
       </c>
-      <c r="K36" s="22">
+      <c r="K36" s="19">
         <v>0.91300000000000003</v>
       </c>
-      <c r="L36" s="22">
+      <c r="L36" s="19">
         <v>0.91400000000000003</v>
       </c>
       <c r="M36" s="11">
@@ -3382,7 +3382,7 @@
         <v>#DIV/0!</v>
       </c>
       <c r="U36" s="15"/>
-      <c r="V36" s="19"/>
+      <c r="V36" s="22"/>
       <c r="W36" s="4" t="s">
         <v>2</v>
       </c>
@@ -3398,13 +3398,13 @@
       <c r="AD36" s="9">
         <v>5922</v>
       </c>
-      <c r="AE36" s="22">
+      <c r="AE36" s="19">
         <v>6307</v>
       </c>
-      <c r="AF36" s="22">
+      <c r="AF36" s="19">
         <v>6444</v>
       </c>
-      <c r="AG36" s="22">
+      <c r="AG36" s="19">
         <v>6437</v>
       </c>
       <c r="AH36" s="11">
@@ -3425,7 +3425,7 @@
       </c>
     </row>
     <row r="37" spans="1:41" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A37" s="19"/>
+      <c r="A37" s="22"/>
       <c r="B37" s="4" t="s">
         <v>3</v>
       </c>
@@ -3441,13 +3441,13 @@
       <c r="I37" s="9">
         <v>2.827</v>
       </c>
-      <c r="J37" s="22">
+      <c r="J37" s="19">
         <v>2.7909999999999999</v>
       </c>
-      <c r="K37" s="22">
+      <c r="K37" s="19">
         <v>2.8109999999999999</v>
       </c>
-      <c r="L37" s="22">
+      <c r="L37" s="19">
         <v>2.786</v>
       </c>
       <c r="M37" s="11">
@@ -3467,7 +3467,7 @@
         <v>#DIV/0!</v>
       </c>
       <c r="U37" s="15"/>
-      <c r="V37" s="19"/>
+      <c r="V37" s="22"/>
       <c r="W37" s="4" t="s">
         <v>3</v>
       </c>
@@ -3483,13 +3483,13 @@
       <c r="AD37" s="9">
         <v>7380</v>
       </c>
-      <c r="AE37" s="22">
+      <c r="AE37" s="19">
         <v>7478</v>
       </c>
-      <c r="AF37" s="22">
+      <c r="AF37" s="19">
         <v>7423</v>
       </c>
-      <c r="AG37" s="22">
+      <c r="AG37" s="19">
         <v>7489</v>
       </c>
       <c r="AH37" s="11">
@@ -3510,7 +3510,7 @@
       </c>
     </row>
     <row r="38" spans="1:41" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A38" s="19"/>
+      <c r="A38" s="22"/>
       <c r="B38" s="4" t="s">
         <v>4</v>
       </c>
@@ -3526,13 +3526,13 @@
       <c r="I38" s="9">
         <v>8.407</v>
       </c>
-      <c r="J38" s="22">
+      <c r="J38" s="19">
         <v>8.3979999999999997</v>
       </c>
-      <c r="K38" s="22">
+      <c r="K38" s="19">
         <v>8.2279999999999998</v>
       </c>
-      <c r="L38" s="22">
+      <c r="L38" s="19">
         <v>8.2129999999999992</v>
       </c>
       <c r="M38" s="11">
@@ -3552,7 +3552,7 @@
         <v>#DIV/0!</v>
       </c>
       <c r="U38" s="15"/>
-      <c r="V38" s="19"/>
+      <c r="V38" s="22"/>
       <c r="W38" s="4" t="s">
         <v>4</v>
       </c>
@@ -3568,13 +3568,13 @@
       <c r="AD38" s="9">
         <v>9849</v>
       </c>
-      <c r="AE38" s="22">
+      <c r="AE38" s="19">
         <v>9860</v>
       </c>
-      <c r="AF38" s="22">
+      <c r="AF38" s="19">
         <v>10060</v>
       </c>
-      <c r="AG38" s="22">
+      <c r="AG38" s="19">
         <v>10080</v>
       </c>
       <c r="AH38" s="11">
@@ -3595,7 +3595,7 @@
       </c>
     </row>
     <row r="39" spans="1:41" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A39" s="19"/>
+      <c r="A39" s="22"/>
       <c r="B39" s="4" t="s">
         <v>5</v>
       </c>
@@ -3611,13 +3611,13 @@
       <c r="I39" s="9">
         <v>14.922000000000001</v>
       </c>
-      <c r="J39" s="22">
+      <c r="J39" s="19">
         <v>14.868</v>
       </c>
-      <c r="K39" s="22">
+      <c r="K39" s="19">
         <v>14.528</v>
       </c>
-      <c r="L39" s="22">
+      <c r="L39" s="19">
         <v>14.657999999999999</v>
       </c>
       <c r="M39" s="11">
@@ -3637,7 +3637,7 @@
         <v>#DIV/0!</v>
       </c>
       <c r="U39" s="15"/>
-      <c r="V39" s="19"/>
+      <c r="V39" s="22"/>
       <c r="W39" s="4" t="s">
         <v>5</v>
       </c>
@@ -3653,13 +3653,13 @@
       <c r="AD39" s="9">
         <v>10820</v>
       </c>
-      <c r="AE39" s="22">
+      <c r="AE39" s="19">
         <v>10860</v>
       </c>
-      <c r="AF39" s="22">
+      <c r="AF39" s="19">
         <v>11110</v>
       </c>
-      <c r="AG39" s="22">
+      <c r="AG39" s="19">
         <v>11010</v>
       </c>
       <c r="AH39" s="11">
@@ -3680,7 +3680,7 @@
       </c>
     </row>
     <row r="40" spans="1:41" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A40" s="19"/>
+      <c r="A40" s="22"/>
       <c r="B40" s="4" t="s">
         <v>6</v>
       </c>
@@ -3696,13 +3696,13 @@
       <c r="I40" s="9">
         <v>0.30399999999999999</v>
       </c>
-      <c r="J40" s="22">
+      <c r="J40" s="19">
         <v>0.27500000000000002</v>
       </c>
-      <c r="K40" s="22">
+      <c r="K40" s="19">
         <v>0.27600000000000002</v>
       </c>
-      <c r="L40" s="22">
+      <c r="L40" s="19">
         <v>0.26100000000000001</v>
       </c>
       <c r="M40" s="11">
@@ -3722,7 +3722,7 @@
         <v>#DIV/0!</v>
       </c>
       <c r="U40" s="15"/>
-      <c r="V40" s="19"/>
+      <c r="V40" s="22"/>
       <c r="W40" s="4" t="s">
         <v>6</v>
       </c>
@@ -3738,13 +3738,13 @@
       <c r="AD40" s="9">
         <v>821.8</v>
       </c>
-      <c r="AE40" s="22">
+      <c r="AE40" s="19">
         <v>909.9</v>
       </c>
-      <c r="AF40" s="22">
+      <c r="AF40" s="19">
         <v>906.5</v>
       </c>
-      <c r="AG40" s="22">
+      <c r="AG40" s="19">
         <v>956.3</v>
       </c>
       <c r="AH40" s="11">
@@ -3765,7 +3765,7 @@
       </c>
     </row>
     <row r="41" spans="1:41" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A41" s="19"/>
+      <c r="A41" s="22"/>
       <c r="B41" s="4" t="s">
         <v>7</v>
       </c>
@@ -3781,13 +3781,13 @@
       <c r="I41" s="9">
         <v>0.32200000000000001</v>
       </c>
-      <c r="J41" s="22">
+      <c r="J41" s="19">
         <v>0.28199999999999997</v>
       </c>
-      <c r="K41" s="22">
+      <c r="K41" s="19">
         <v>0.29399999999999998</v>
       </c>
-      <c r="L41" s="22">
+      <c r="L41" s="19">
         <v>0.28899999999999998</v>
       </c>
       <c r="M41" s="11">
@@ -3807,7 +3807,7 @@
         <v>#DIV/0!</v>
       </c>
       <c r="U41" s="15"/>
-      <c r="V41" s="19"/>
+      <c r="V41" s="22"/>
       <c r="W41" s="4" t="s">
         <v>7</v>
       </c>
@@ -3823,13 +3823,13 @@
       <c r="AD41" s="9">
         <v>1552</v>
       </c>
-      <c r="AE41" s="22">
+      <c r="AE41" s="19">
         <v>1771</v>
       </c>
-      <c r="AF41" s="22">
+      <c r="AF41" s="19">
         <v>1697</v>
       </c>
-      <c r="AG41" s="22">
+      <c r="AG41" s="19">
         <v>1730</v>
       </c>
       <c r="AH41" s="11">
@@ -3850,7 +3850,7 @@
       </c>
     </row>
     <row r="42" spans="1:41" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A42" s="19"/>
+      <c r="A42" s="22"/>
       <c r="B42" s="4" t="s">
         <v>8</v>
       </c>
@@ -3866,13 +3866,13 @@
       <c r="I42" s="9">
         <v>0.33</v>
       </c>
-      <c r="J42" s="22">
+      <c r="J42" s="19">
         <v>0.31</v>
       </c>
-      <c r="K42" s="22">
+      <c r="K42" s="19">
         <v>0.26600000000000001</v>
       </c>
-      <c r="L42" s="22">
+      <c r="L42" s="19">
         <v>0.30099999999999999</v>
       </c>
       <c r="M42" s="11">
@@ -3892,7 +3892,7 @@
         <v>#DIV/0!</v>
       </c>
       <c r="U42" s="15"/>
-      <c r="V42" s="19"/>
+      <c r="V42" s="22"/>
       <c r="W42" s="4" t="s">
         <v>8</v>
       </c>
@@ -3908,13 +3908,13 @@
       <c r="AD42" s="9">
         <v>2270</v>
       </c>
-      <c r="AE42" s="22">
+      <c r="AE42" s="19">
         <v>2419</v>
       </c>
-      <c r="AF42" s="22">
+      <c r="AF42" s="19">
         <v>2819</v>
       </c>
-      <c r="AG42" s="22">
+      <c r="AG42" s="19">
         <v>2488</v>
       </c>
       <c r="AH42" s="11">
@@ -3935,7 +3935,7 @@
       </c>
     </row>
     <row r="43" spans="1:41" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A43" s="19"/>
+      <c r="A43" s="22"/>
       <c r="B43" s="4" t="s">
         <v>9</v>
       </c>
@@ -3977,7 +3977,7 @@
         <v>#DIV/0!</v>
       </c>
       <c r="U43" s="15"/>
-      <c r="V43" s="19"/>
+      <c r="V43" s="22"/>
       <c r="W43" s="4" t="s">
         <v>9</v>
       </c>
@@ -4063,7 +4063,7 @@
       <c r="AO44" s="15"/>
     </row>
     <row r="45" spans="1:41" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A45" s="19" t="s">
+      <c r="A45" s="22" t="s">
         <v>23</v>
       </c>
       <c r="B45" s="4" t="s">
@@ -4078,14 +4078,24 @@
         <f>AVERAGE(C45:G45)</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="I45" s="6"/>
-      <c r="J45" s="7"/>
-      <c r="K45" s="7"/>
-      <c r="L45" s="7"/>
-      <c r="M45" s="8"/>
-      <c r="N45" s="5" t="e">
+      <c r="I45" s="6">
+        <v>0.34300000000000003</v>
+      </c>
+      <c r="J45" s="7">
+        <v>0.28399999999999997</v>
+      </c>
+      <c r="K45" s="7">
+        <v>0.28799999999999998</v>
+      </c>
+      <c r="L45" s="7">
+        <v>0.27600000000000002</v>
+      </c>
+      <c r="M45" s="8">
+        <v>0.28999999999999998</v>
+      </c>
+      <c r="N45" s="5">
         <f>AVERAGE(I45:M45)</f>
-        <v>#DIV/0!</v>
+        <v>0.29620000000000002</v>
       </c>
       <c r="O45" s="6"/>
       <c r="P45" s="7"/>
@@ -4097,7 +4107,7 @@
         <v>#DIV/0!</v>
       </c>
       <c r="U45" s="15"/>
-      <c r="V45" s="19" t="s">
+      <c r="V45" s="22" t="s">
         <v>23</v>
       </c>
       <c r="W45" s="4" t="s">
@@ -4112,14 +4122,24 @@
         <f>AVERAGE(X45:AB45)</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="AD45" s="6"/>
-      <c r="AE45" s="7"/>
-      <c r="AF45" s="7"/>
-      <c r="AG45" s="7"/>
-      <c r="AH45" s="8"/>
-      <c r="AI45" s="5" t="e">
+      <c r="AD45" s="6">
+        <v>86.64</v>
+      </c>
+      <c r="AE45" s="7">
+        <v>104.7</v>
+      </c>
+      <c r="AF45" s="7">
+        <v>103.1</v>
+      </c>
+      <c r="AG45" s="7">
+        <v>107.5</v>
+      </c>
+      <c r="AH45" s="8">
+        <v>102.5</v>
+      </c>
+      <c r="AI45" s="5">
         <f>AVERAGE(AD45:AH45)</f>
-        <v>#DIV/0!</v>
+        <v>100.88800000000001</v>
       </c>
       <c r="AJ45" s="6"/>
       <c r="AK45" s="7"/>
@@ -4132,7 +4152,7 @@
       </c>
     </row>
     <row r="46" spans="1:41" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A46" s="19"/>
+      <c r="A46" s="22"/>
       <c r="B46" s="4" t="s">
         <v>2</v>
       </c>
@@ -4145,14 +4165,24 @@
         <f t="shared" ref="H46:H53" si="24">AVERAGE(C46:G46)</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="I46" s="9"/>
-      <c r="J46" s="10"/>
-      <c r="K46" s="10"/>
-      <c r="L46" s="10"/>
-      <c r="M46" s="11"/>
-      <c r="N46" s="5" t="e">
+      <c r="I46" s="9">
+        <v>1.0009999999999999</v>
+      </c>
+      <c r="J46" s="19">
+        <v>0.92</v>
+      </c>
+      <c r="K46" s="19">
+        <v>0.93400000000000005</v>
+      </c>
+      <c r="L46" s="19">
+        <v>0.95299999999999996</v>
+      </c>
+      <c r="M46" s="11">
+        <v>0.93500000000000005</v>
+      </c>
+      <c r="N46" s="5">
         <f t="shared" ref="N46:N53" si="25">AVERAGE(I46:M46)</f>
-        <v>#DIV/0!</v>
+        <v>0.94860000000000011</v>
       </c>
       <c r="O46" s="9"/>
       <c r="P46" s="10"/>
@@ -4164,7 +4194,7 @@
         <v>#DIV/0!</v>
       </c>
       <c r="U46" s="15"/>
-      <c r="V46" s="19"/>
+      <c r="V46" s="22"/>
       <c r="W46" s="4" t="s">
         <v>2</v>
       </c>
@@ -4177,14 +4207,24 @@
         <f t="shared" ref="AC46:AC53" si="27">AVERAGE(X46:AB46)</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="AD46" s="9"/>
-      <c r="AE46" s="10"/>
-      <c r="AF46" s="10"/>
-      <c r="AG46" s="10"/>
-      <c r="AH46" s="11"/>
-      <c r="AI46" s="5" t="e">
+      <c r="AD46" s="9">
+        <v>5873</v>
+      </c>
+      <c r="AE46" s="19">
+        <v>6393</v>
+      </c>
+      <c r="AF46" s="19">
+        <v>6295</v>
+      </c>
+      <c r="AG46" s="19">
+        <v>6174</v>
+      </c>
+      <c r="AH46" s="11">
+        <v>6286</v>
+      </c>
+      <c r="AI46" s="5">
         <f t="shared" ref="AI46:AI53" si="28">AVERAGE(AD46:AH46)</f>
-        <v>#DIV/0!</v>
+        <v>6204.2</v>
       </c>
       <c r="AJ46" s="9"/>
       <c r="AK46" s="10"/>
@@ -4197,7 +4237,7 @@
       </c>
     </row>
     <row r="47" spans="1:41" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A47" s="19"/>
+      <c r="A47" s="22"/>
       <c r="B47" s="4" t="s">
         <v>3</v>
       </c>
@@ -4210,14 +4250,24 @@
         <f t="shared" si="24"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="I47" s="9"/>
-      <c r="J47" s="10"/>
-      <c r="K47" s="10"/>
-      <c r="L47" s="10"/>
-      <c r="M47" s="11"/>
-      <c r="N47" s="5" t="e">
+      <c r="I47" s="9">
+        <v>2.8740000000000001</v>
+      </c>
+      <c r="J47" s="19">
+        <v>2.77</v>
+      </c>
+      <c r="K47" s="19">
+        <v>2.7759999999999998</v>
+      </c>
+      <c r="L47" s="19">
+        <v>2.7120000000000002</v>
+      </c>
+      <c r="M47" s="11">
+        <v>2.7629999999999999</v>
+      </c>
+      <c r="N47" s="5">
         <f t="shared" si="25"/>
-        <v>#DIV/0!</v>
+        <v>2.7789999999999999</v>
       </c>
       <c r="O47" s="9"/>
       <c r="P47" s="10"/>
@@ -4229,7 +4279,7 @@
         <v>#DIV/0!</v>
       </c>
       <c r="U47" s="15"/>
-      <c r="V47" s="19"/>
+      <c r="V47" s="22"/>
       <c r="W47" s="4" t="s">
         <v>3</v>
       </c>
@@ -4242,14 +4292,24 @@
         <f t="shared" si="27"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="AD47" s="9"/>
-      <c r="AE47" s="10"/>
-      <c r="AF47" s="10"/>
-      <c r="AG47" s="10"/>
-      <c r="AH47" s="11"/>
-      <c r="AI47" s="5" t="e">
+      <c r="AD47" s="9">
+        <v>7260</v>
+      </c>
+      <c r="AE47" s="19">
+        <v>7534</v>
+      </c>
+      <c r="AF47" s="19">
+        <v>7515</v>
+      </c>
+      <c r="AG47" s="19">
+        <v>7694</v>
+      </c>
+      <c r="AH47" s="11">
+        <v>7553</v>
+      </c>
+      <c r="AI47" s="5">
         <f t="shared" si="28"/>
-        <v>#DIV/0!</v>
+        <v>7511.2</v>
       </c>
       <c r="AJ47" s="9"/>
       <c r="AK47" s="10"/>
@@ -4262,7 +4322,7 @@
       </c>
     </row>
     <row r="48" spans="1:41" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A48" s="19"/>
+      <c r="A48" s="22"/>
       <c r="B48" s="4" t="s">
         <v>4</v>
       </c>
@@ -4275,14 +4335,24 @@
         <f t="shared" si="24"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="I48" s="9"/>
-      <c r="J48" s="10"/>
-      <c r="K48" s="10"/>
-      <c r="L48" s="10"/>
-      <c r="M48" s="11"/>
-      <c r="N48" s="5" t="e">
+      <c r="I48" s="9">
+        <v>8.5570000000000004</v>
+      </c>
+      <c r="J48" s="19">
+        <v>8.4540000000000006</v>
+      </c>
+      <c r="K48" s="19">
+        <v>8.4380000000000006</v>
+      </c>
+      <c r="L48" s="19">
+        <v>8.3420000000000005</v>
+      </c>
+      <c r="M48" s="11">
+        <v>8.4890000000000008</v>
+      </c>
+      <c r="N48" s="5">
         <f t="shared" si="25"/>
-        <v>#DIV/0!</v>
+        <v>8.4559999999999995</v>
       </c>
       <c r="O48" s="9"/>
       <c r="P48" s="10"/>
@@ -4294,7 +4364,7 @@
         <v>#DIV/0!</v>
       </c>
       <c r="U48" s="15"/>
-      <c r="V48" s="19"/>
+      <c r="V48" s="22"/>
       <c r="W48" s="4" t="s">
         <v>4</v>
       </c>
@@ -4307,14 +4377,24 @@
         <f t="shared" si="27"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="AD48" s="9"/>
-      <c r="AE48" s="10"/>
-      <c r="AF48" s="10"/>
-      <c r="AG48" s="10"/>
-      <c r="AH48" s="11"/>
-      <c r="AI48" s="5" t="e">
+      <c r="AD48" s="9">
+        <v>9676</v>
+      </c>
+      <c r="AE48" s="19">
+        <v>9795</v>
+      </c>
+      <c r="AF48" s="19">
+        <v>9813</v>
+      </c>
+      <c r="AG48" s="19">
+        <v>9926</v>
+      </c>
+      <c r="AH48" s="11">
+        <v>9754</v>
+      </c>
+      <c r="AI48" s="5">
         <f t="shared" si="28"/>
-        <v>#DIV/0!</v>
+        <v>9792.7999999999993</v>
       </c>
       <c r="AJ48" s="9"/>
       <c r="AK48" s="10"/>
@@ -4327,7 +4407,7 @@
       </c>
     </row>
     <row r="49" spans="1:41" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A49" s="19"/>
+      <c r="A49" s="22"/>
       <c r="B49" s="4" t="s">
         <v>5</v>
       </c>
@@ -4340,14 +4420,24 @@
         <f t="shared" si="24"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="I49" s="9"/>
-      <c r="J49" s="10"/>
-      <c r="K49" s="10"/>
-      <c r="L49" s="10"/>
-      <c r="M49" s="11"/>
-      <c r="N49" s="5" t="e">
+      <c r="I49" s="9">
+        <v>15.164999999999999</v>
+      </c>
+      <c r="J49" s="19">
+        <v>14.956</v>
+      </c>
+      <c r="K49" s="19">
+        <v>15.156000000000001</v>
+      </c>
+      <c r="L49" s="19">
+        <v>15.005000000000001</v>
+      </c>
+      <c r="M49" s="11">
+        <v>15.19</v>
+      </c>
+      <c r="N49" s="5">
         <f t="shared" si="25"/>
-        <v>#DIV/0!</v>
+        <v>15.094400000000002</v>
       </c>
       <c r="O49" s="9"/>
       <c r="P49" s="10"/>
@@ -4359,7 +4449,7 @@
         <v>#DIV/0!</v>
       </c>
       <c r="U49" s="15"/>
-      <c r="V49" s="19"/>
+      <c r="V49" s="22"/>
       <c r="W49" s="4" t="s">
         <v>5</v>
       </c>
@@ -4372,14 +4462,24 @@
         <f t="shared" si="27"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="AD49" s="9"/>
-      <c r="AE49" s="10"/>
-      <c r="AF49" s="10"/>
-      <c r="AG49" s="10"/>
-      <c r="AH49" s="11"/>
-      <c r="AI49" s="5" t="e">
+      <c r="AD49" s="9">
+        <v>10650</v>
+      </c>
+      <c r="AE49" s="19">
+        <v>10790</v>
+      </c>
+      <c r="AF49" s="19">
+        <v>10650</v>
+      </c>
+      <c r="AG49" s="19">
+        <v>10760</v>
+      </c>
+      <c r="AH49" s="11">
+        <v>10630</v>
+      </c>
+      <c r="AI49" s="5">
         <f t="shared" si="28"/>
-        <v>#DIV/0!</v>
+        <v>10696</v>
       </c>
       <c r="AJ49" s="9"/>
       <c r="AK49" s="10"/>
@@ -4392,7 +4492,7 @@
       </c>
     </row>
     <row r="50" spans="1:41" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A50" s="19"/>
+      <c r="A50" s="22"/>
       <c r="B50" s="4" t="s">
         <v>6</v>
       </c>
@@ -4405,14 +4505,24 @@
         <f t="shared" si="24"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="I50" s="9"/>
-      <c r="J50" s="10"/>
-      <c r="K50" s="10"/>
-      <c r="L50" s="10"/>
-      <c r="M50" s="11"/>
-      <c r="N50" s="5" t="e">
+      <c r="I50" s="9">
+        <v>0.30599999999999999</v>
+      </c>
+      <c r="J50" s="19">
+        <v>0.27600000000000002</v>
+      </c>
+      <c r="K50" s="19">
+        <v>0.28999999999999998</v>
+      </c>
+      <c r="L50" s="19">
+        <v>0.28000000000000003</v>
+      </c>
+      <c r="M50" s="11">
+        <v>0.26200000000000001</v>
+      </c>
+      <c r="N50" s="5">
         <f t="shared" si="25"/>
-        <v>#DIV/0!</v>
+        <v>0.28280000000000005</v>
       </c>
       <c r="O50" s="9"/>
       <c r="P50" s="10"/>
@@ -4424,7 +4534,7 @@
         <v>#DIV/0!</v>
       </c>
       <c r="U50" s="15"/>
-      <c r="V50" s="19"/>
+      <c r="V50" s="22"/>
       <c r="W50" s="4" t="s">
         <v>6</v>
       </c>
@@ -4437,14 +4547,24 @@
         <f t="shared" si="27"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="AD50" s="9"/>
-      <c r="AE50" s="10"/>
-      <c r="AF50" s="10"/>
-      <c r="AG50" s="10"/>
-      <c r="AH50" s="11"/>
-      <c r="AI50" s="5" t="e">
+      <c r="AD50" s="9">
+        <v>816.7</v>
+      </c>
+      <c r="AE50" s="19">
+        <v>903.7</v>
+      </c>
+      <c r="AF50" s="19">
+        <v>860.8</v>
+      </c>
+      <c r="AG50" s="19">
+        <v>890.6</v>
+      </c>
+      <c r="AH50" s="11">
+        <v>954.2</v>
+      </c>
+      <c r="AI50" s="5">
         <f t="shared" si="28"/>
-        <v>#DIV/0!</v>
+        <v>885.2</v>
       </c>
       <c r="AJ50" s="9"/>
       <c r="AK50" s="10"/>
@@ -4457,7 +4577,7 @@
       </c>
     </row>
     <row r="51" spans="1:41" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A51" s="19"/>
+      <c r="A51" s="22"/>
       <c r="B51" s="4" t="s">
         <v>7</v>
       </c>
@@ -4470,14 +4590,24 @@
         <f t="shared" si="24"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="I51" s="9"/>
-      <c r="J51" s="10"/>
-      <c r="K51" s="10"/>
-      <c r="L51" s="10"/>
-      <c r="M51" s="11"/>
-      <c r="N51" s="5" t="e">
+      <c r="I51" s="9">
+        <v>0.312</v>
+      </c>
+      <c r="J51" s="19">
+        <v>0.28499999999999998</v>
+      </c>
+      <c r="K51" s="19">
+        <v>0.28499999999999998</v>
+      </c>
+      <c r="L51" s="19">
+        <v>0.28699999999999998</v>
+      </c>
+      <c r="M51" s="11">
+        <v>0.29199999999999998</v>
+      </c>
+      <c r="N51" s="5">
         <f t="shared" si="25"/>
-        <v>#DIV/0!</v>
+        <v>0.29219999999999996</v>
       </c>
       <c r="O51" s="9"/>
       <c r="P51" s="10"/>
@@ -4489,7 +4619,7 @@
         <v>#DIV/0!</v>
       </c>
       <c r="U51" s="15"/>
-      <c r="V51" s="19"/>
+      <c r="V51" s="22"/>
       <c r="W51" s="4" t="s">
         <v>7</v>
       </c>
@@ -4502,14 +4632,24 @@
         <f t="shared" si="27"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="AD51" s="9"/>
-      <c r="AE51" s="10"/>
-      <c r="AF51" s="10"/>
-      <c r="AG51" s="10"/>
-      <c r="AH51" s="11"/>
-      <c r="AI51" s="5" t="e">
+      <c r="AD51" s="9">
+        <v>1603</v>
+      </c>
+      <c r="AE51" s="19">
+        <v>1756</v>
+      </c>
+      <c r="AF51" s="19">
+        <v>1751</v>
+      </c>
+      <c r="AG51" s="19">
+        <v>1741</v>
+      </c>
+      <c r="AH51" s="11">
+        <v>1713</v>
+      </c>
+      <c r="AI51" s="5">
         <f t="shared" si="28"/>
-        <v>#DIV/0!</v>
+        <v>1712.8</v>
       </c>
       <c r="AJ51" s="9"/>
       <c r="AK51" s="10"/>
@@ -4522,7 +4662,7 @@
       </c>
     </row>
     <row r="52" spans="1:41" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A52" s="19"/>
+      <c r="A52" s="22"/>
       <c r="B52" s="4" t="s">
         <v>8</v>
       </c>
@@ -4535,14 +4675,24 @@
         <f t="shared" si="24"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="I52" s="9"/>
-      <c r="J52" s="10"/>
-      <c r="K52" s="10"/>
-      <c r="L52" s="10"/>
-      <c r="M52" s="11"/>
-      <c r="N52" s="5" t="e">
+      <c r="I52" s="9">
+        <v>0.32100000000000001</v>
+      </c>
+      <c r="J52" s="19">
+        <v>0.28999999999999998</v>
+      </c>
+      <c r="K52" s="19">
+        <v>0.30399999999999999</v>
+      </c>
+      <c r="L52" s="19">
+        <v>0.31</v>
+      </c>
+      <c r="M52" s="11">
+        <v>0.313</v>
+      </c>
+      <c r="N52" s="5">
         <f t="shared" si="25"/>
-        <v>#DIV/0!</v>
+        <v>0.30759999999999998</v>
       </c>
       <c r="O52" s="9"/>
       <c r="P52" s="10"/>
@@ -4554,7 +4704,7 @@
         <v>#DIV/0!</v>
       </c>
       <c r="U52" s="15"/>
-      <c r="V52" s="19"/>
+      <c r="V52" s="22"/>
       <c r="W52" s="4" t="s">
         <v>8</v>
       </c>
@@ -4567,14 +4717,24 @@
         <f t="shared" si="27"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="AD52" s="9"/>
-      <c r="AE52" s="10"/>
-      <c r="AF52" s="10"/>
-      <c r="AG52" s="10"/>
-      <c r="AH52" s="11"/>
-      <c r="AI52" s="5" t="e">
+      <c r="AD52" s="9">
+        <v>2332</v>
+      </c>
+      <c r="AE52" s="19">
+        <v>2583</v>
+      </c>
+      <c r="AF52" s="19">
+        <v>2465</v>
+      </c>
+      <c r="AG52" s="19">
+        <v>2414</v>
+      </c>
+      <c r="AH52" s="11">
+        <v>2395</v>
+      </c>
+      <c r="AI52" s="5">
         <f t="shared" si="28"/>
-        <v>#DIV/0!</v>
+        <v>2437.8000000000002</v>
       </c>
       <c r="AJ52" s="9"/>
       <c r="AK52" s="10"/>
@@ -4587,7 +4747,7 @@
       </c>
     </row>
     <row r="53" spans="1:41" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A53" s="19"/>
+      <c r="A53" s="22"/>
       <c r="B53" s="4" t="s">
         <v>9</v>
       </c>
@@ -4600,14 +4760,24 @@
         <f t="shared" si="24"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="I53" s="12"/>
-      <c r="J53" s="13"/>
-      <c r="K53" s="13"/>
-      <c r="L53" s="13"/>
-      <c r="M53" s="14"/>
-      <c r="N53" s="5" t="e">
+      <c r="I53" s="12">
+        <v>0.34300000000000003</v>
+      </c>
+      <c r="J53" s="13">
+        <v>0.312</v>
+      </c>
+      <c r="K53" s="13">
+        <v>0.307</v>
+      </c>
+      <c r="L53" s="13">
+        <v>0.30599999999999999</v>
+      </c>
+      <c r="M53" s="14">
+        <v>0.30199999999999999</v>
+      </c>
+      <c r="N53" s="5">
         <f t="shared" si="25"/>
-        <v>#DIV/0!</v>
+        <v>0.314</v>
       </c>
       <c r="O53" s="12"/>
       <c r="P53" s="13"/>
@@ -4619,7 +4789,7 @@
         <v>#DIV/0!</v>
       </c>
       <c r="U53" s="15"/>
-      <c r="V53" s="19"/>
+      <c r="V53" s="22"/>
       <c r="W53" s="4" t="s">
         <v>9</v>
       </c>
@@ -4632,14 +4802,24 @@
         <f t="shared" si="27"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="AD53" s="12"/>
-      <c r="AE53" s="13"/>
-      <c r="AF53" s="13"/>
-      <c r="AG53" s="13"/>
-      <c r="AH53" s="14"/>
-      <c r="AI53" s="5" t="e">
+      <c r="AD53" s="12">
+        <v>2916</v>
+      </c>
+      <c r="AE53" s="13">
+        <v>3203</v>
+      </c>
+      <c r="AF53" s="13">
+        <v>3249</v>
+      </c>
+      <c r="AG53" s="13">
+        <v>3263</v>
+      </c>
+      <c r="AH53" s="14">
+        <v>3310</v>
+      </c>
+      <c r="AI53" s="5">
         <f t="shared" si="28"/>
-        <v>#DIV/0!</v>
+        <v>3188.2</v>
       </c>
       <c r="AJ53" s="12"/>
       <c r="AK53" s="13"/>
@@ -4695,7 +4875,7 @@
       <c r="AO54" s="15"/>
     </row>
     <row r="55" spans="1:41" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A55" s="19" t="s">
+      <c r="A55" s="22" t="s">
         <v>24</v>
       </c>
       <c r="B55" s="4" t="s">
@@ -4710,14 +4890,24 @@
         <f>AVERAGE(C55:G55)</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="I55" s="6"/>
-      <c r="J55" s="7"/>
-      <c r="K55" s="7"/>
-      <c r="L55" s="7"/>
-      <c r="M55" s="8"/>
-      <c r="N55" s="5" t="e">
+      <c r="I55" s="6">
+        <v>0.36899999999999999</v>
+      </c>
+      <c r="J55" s="7">
+        <v>0.28799999999999998</v>
+      </c>
+      <c r="K55" s="7">
+        <v>0.29199999999999998</v>
+      </c>
+      <c r="L55" s="7">
+        <v>0.28699999999999998</v>
+      </c>
+      <c r="M55" s="8">
+        <v>0.27300000000000002</v>
+      </c>
+      <c r="N55" s="5">
         <f>AVERAGE(I55:M55)</f>
-        <v>#DIV/0!</v>
+        <v>0.30179999999999996</v>
       </c>
       <c r="O55" s="6"/>
       <c r="P55" s="7"/>
@@ -4729,7 +4919,7 @@
         <v>#DIV/0!</v>
       </c>
       <c r="U55" s="15"/>
-      <c r="V55" s="19" t="s">
+      <c r="V55" s="22" t="s">
         <v>24</v>
       </c>
       <c r="W55" s="4" t="s">
@@ -4744,14 +4934,24 @@
         <f>AVERAGE(X55:AB55)</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="AD55" s="6"/>
-      <c r="AE55" s="7"/>
-      <c r="AF55" s="7"/>
-      <c r="AG55" s="7"/>
-      <c r="AH55" s="8"/>
-      <c r="AI55" s="5" t="e">
+      <c r="AD55" s="6">
+        <v>80.459999999999994</v>
+      </c>
+      <c r="AE55" s="7">
+        <v>103.1</v>
+      </c>
+      <c r="AF55" s="7">
+        <v>101.6</v>
+      </c>
+      <c r="AG55" s="7">
+        <v>103.3</v>
+      </c>
+      <c r="AH55" s="8">
+        <v>109</v>
+      </c>
+      <c r="AI55" s="5">
         <f>AVERAGE(AD55:AH55)</f>
-        <v>#DIV/0!</v>
+        <v>99.49199999999999</v>
       </c>
       <c r="AJ55" s="6"/>
       <c r="AK55" s="7"/>
@@ -4764,7 +4964,7 @@
       </c>
     </row>
     <row r="56" spans="1:41" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A56" s="19"/>
+      <c r="A56" s="22"/>
       <c r="B56" s="4" t="s">
         <v>2</v>
       </c>
@@ -4777,14 +4977,24 @@
         <f t="shared" ref="H56:H63" si="30">AVERAGE(C56:G56)</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="I56" s="9"/>
-      <c r="J56" s="10"/>
-      <c r="K56" s="10"/>
-      <c r="L56" s="10"/>
-      <c r="M56" s="11"/>
-      <c r="N56" s="5" t="e">
+      <c r="I56" s="9">
+        <v>1.032</v>
+      </c>
+      <c r="J56" s="19">
+        <v>0.99199999999999999</v>
+      </c>
+      <c r="K56" s="19">
+        <v>0.99299999999999999</v>
+      </c>
+      <c r="L56" s="19">
+        <v>0.98199999999999998</v>
+      </c>
+      <c r="M56" s="11">
+        <v>0.93899999999999995</v>
+      </c>
+      <c r="N56" s="5">
         <f t="shared" ref="N56:N63" si="31">AVERAGE(I56:M56)</f>
-        <v>#DIV/0!</v>
+        <v>0.98759999999999992</v>
       </c>
       <c r="O56" s="9"/>
       <c r="P56" s="10"/>
@@ -4796,7 +5006,7 @@
         <v>#DIV/0!</v>
       </c>
       <c r="U56" s="15"/>
-      <c r="V56" s="19"/>
+      <c r="V56" s="22"/>
       <c r="W56" s="4" t="s">
         <v>2</v>
       </c>
@@ -4809,14 +5019,24 @@
         <f t="shared" ref="AC56:AC63" si="33">AVERAGE(X56:AB56)</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="AD56" s="9"/>
-      <c r="AE56" s="10"/>
-      <c r="AF56" s="10"/>
-      <c r="AG56" s="10"/>
-      <c r="AH56" s="11"/>
-      <c r="AI56" s="5" t="e">
+      <c r="AD56" s="9">
+        <v>5696</v>
+      </c>
+      <c r="AE56" s="19">
+        <v>5930</v>
+      </c>
+      <c r="AF56" s="19">
+        <v>5920</v>
+      </c>
+      <c r="AG56" s="19">
+        <v>5987</v>
+      </c>
+      <c r="AH56" s="11">
+        <v>6261</v>
+      </c>
+      <c r="AI56" s="5">
         <f t="shared" ref="AI56:AI63" si="34">AVERAGE(AD56:AH56)</f>
-        <v>#DIV/0!</v>
+        <v>5958.8</v>
       </c>
       <c r="AJ56" s="9"/>
       <c r="AK56" s="10"/>
@@ -4829,7 +5049,7 @@
       </c>
     </row>
     <row r="57" spans="1:41" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A57" s="19"/>
+      <c r="A57" s="22"/>
       <c r="B57" s="4" t="s">
         <v>3</v>
       </c>
@@ -4842,14 +5062,24 @@
         <f t="shared" si="30"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="I57" s="9"/>
-      <c r="J57" s="10"/>
-      <c r="K57" s="10"/>
-      <c r="L57" s="10"/>
-      <c r="M57" s="11"/>
-      <c r="N57" s="5" t="e">
+      <c r="I57" s="9">
+        <v>2.7669999999999999</v>
+      </c>
+      <c r="J57" s="19">
+        <v>2.7629999999999999</v>
+      </c>
+      <c r="K57" s="19">
+        <v>2.782</v>
+      </c>
+      <c r="L57" s="19">
+        <v>2.7559999999999998</v>
+      </c>
+      <c r="M57" s="11">
+        <v>2.7959999999999998</v>
+      </c>
+      <c r="N57" s="5">
         <f t="shared" si="31"/>
-        <v>#DIV/0!</v>
+        <v>2.7727999999999997</v>
       </c>
       <c r="O57" s="9"/>
       <c r="P57" s="10"/>
@@ -4861,7 +5091,7 @@
         <v>#DIV/0!</v>
       </c>
       <c r="U57" s="15"/>
-      <c r="V57" s="19"/>
+      <c r="V57" s="22"/>
       <c r="W57" s="4" t="s">
         <v>3</v>
       </c>
@@ -4874,14 +5104,24 @@
         <f t="shared" si="33"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="AD57" s="9"/>
-      <c r="AE57" s="10"/>
-      <c r="AF57" s="10"/>
-      <c r="AG57" s="10"/>
-      <c r="AH57" s="11"/>
-      <c r="AI57" s="5" t="e">
+      <c r="AD57" s="9">
+        <v>7542</v>
+      </c>
+      <c r="AE57" s="19">
+        <v>7551</v>
+      </c>
+      <c r="AF57" s="19">
+        <v>7500</v>
+      </c>
+      <c r="AG57" s="19">
+        <v>7572</v>
+      </c>
+      <c r="AH57" s="11">
+        <v>7464</v>
+      </c>
+      <c r="AI57" s="5">
         <f t="shared" si="34"/>
-        <v>#DIV/0!</v>
+        <v>7525.8</v>
       </c>
       <c r="AJ57" s="9"/>
       <c r="AK57" s="10"/>
@@ -4894,7 +5134,7 @@
       </c>
     </row>
     <row r="58" spans="1:41" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A58" s="19"/>
+      <c r="A58" s="22"/>
       <c r="B58" s="4" t="s">
         <v>4</v>
       </c>
@@ -4907,14 +5147,24 @@
         <f t="shared" si="30"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="I58" s="9"/>
-      <c r="J58" s="10"/>
-      <c r="K58" s="10"/>
-      <c r="L58" s="10"/>
-      <c r="M58" s="11"/>
-      <c r="N58" s="5" t="e">
+      <c r="I58" s="9">
+        <v>8.1989999999999998</v>
+      </c>
+      <c r="J58" s="19">
+        <v>8.375</v>
+      </c>
+      <c r="K58" s="19">
+        <v>8.1319999999999997</v>
+      </c>
+      <c r="L58" s="19">
+        <v>8.3409999999999993</v>
+      </c>
+      <c r="M58" s="11">
+        <v>8.2230000000000008</v>
+      </c>
+      <c r="N58" s="5">
         <f t="shared" si="31"/>
-        <v>#DIV/0!</v>
+        <v>8.2539999999999996</v>
       </c>
       <c r="O58" s="9"/>
       <c r="P58" s="10"/>
@@ -4926,7 +5176,7 @@
         <v>#DIV/0!</v>
       </c>
       <c r="U58" s="15"/>
-      <c r="V58" s="19"/>
+      <c r="V58" s="22"/>
       <c r="W58" s="4" t="s">
         <v>4</v>
       </c>
@@ -4939,14 +5189,24 @@
         <f t="shared" si="33"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="AD58" s="9"/>
-      <c r="AE58" s="10"/>
-      <c r="AF58" s="10"/>
-      <c r="AG58" s="10"/>
-      <c r="AH58" s="11"/>
-      <c r="AI58" s="5" t="e">
+      <c r="AD58" s="9">
+        <v>10100</v>
+      </c>
+      <c r="AE58" s="19">
+        <v>9887</v>
+      </c>
+      <c r="AF58" s="19">
+        <v>10180</v>
+      </c>
+      <c r="AG58" s="19">
+        <v>9927</v>
+      </c>
+      <c r="AH58" s="11">
+        <v>10070</v>
+      </c>
+      <c r="AI58" s="5">
         <f t="shared" si="34"/>
-        <v>#DIV/0!</v>
+        <v>10032.799999999999</v>
       </c>
       <c r="AJ58" s="9"/>
       <c r="AK58" s="10"/>
@@ -4959,7 +5219,7 @@
       </c>
     </row>
     <row r="59" spans="1:41" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A59" s="19"/>
+      <c r="A59" s="22"/>
       <c r="B59" s="4" t="s">
         <v>5</v>
       </c>
@@ -4972,14 +5232,24 @@
         <f t="shared" si="30"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="I59" s="9"/>
-      <c r="J59" s="10"/>
-      <c r="K59" s="10"/>
-      <c r="L59" s="10"/>
-      <c r="M59" s="11"/>
-      <c r="N59" s="5" t="e">
+      <c r="I59" s="9">
+        <v>14.372999999999999</v>
+      </c>
+      <c r="J59" s="19">
+        <v>14.584</v>
+      </c>
+      <c r="K59" s="19">
+        <v>14.327</v>
+      </c>
+      <c r="L59" s="19">
+        <v>14.542999999999999</v>
+      </c>
+      <c r="M59" s="11">
+        <v>14.375</v>
+      </c>
+      <c r="N59" s="5">
         <f t="shared" si="31"/>
-        <v>#DIV/0!</v>
+        <v>14.4404</v>
       </c>
       <c r="O59" s="9"/>
       <c r="P59" s="10"/>
@@ -4991,7 +5261,7 @@
         <v>#DIV/0!</v>
       </c>
       <c r="U59" s="15"/>
-      <c r="V59" s="19"/>
+      <c r="V59" s="22"/>
       <c r="W59" s="4" t="s">
         <v>5</v>
       </c>
@@ -5004,14 +5274,24 @@
         <f t="shared" si="33"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="AD59" s="9"/>
-      <c r="AE59" s="10"/>
-      <c r="AF59" s="10"/>
-      <c r="AG59" s="10"/>
-      <c r="AH59" s="11"/>
-      <c r="AI59" s="5" t="e">
+      <c r="AD59" s="9">
+        <v>11230</v>
+      </c>
+      <c r="AE59" s="19">
+        <v>11070</v>
+      </c>
+      <c r="AF59" s="19">
+        <v>11270</v>
+      </c>
+      <c r="AG59" s="19">
+        <v>11100</v>
+      </c>
+      <c r="AH59" s="11">
+        <v>11230</v>
+      </c>
+      <c r="AI59" s="5">
         <f t="shared" si="34"/>
-        <v>#DIV/0!</v>
+        <v>11180</v>
       </c>
       <c r="AJ59" s="9"/>
       <c r="AK59" s="10"/>
@@ -5024,7 +5304,7 @@
       </c>
     </row>
     <row r="60" spans="1:41" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A60" s="19"/>
+      <c r="A60" s="22"/>
       <c r="B60" s="4" t="s">
         <v>6</v>
       </c>
@@ -5037,14 +5317,24 @@
         <f t="shared" si="30"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="I60" s="9"/>
-      <c r="J60" s="10"/>
-      <c r="K60" s="10"/>
-      <c r="L60" s="10"/>
-      <c r="M60" s="11"/>
-      <c r="N60" s="5" t="e">
+      <c r="I60" s="9">
+        <v>0.27100000000000002</v>
+      </c>
+      <c r="J60" s="19">
+        <v>0.28000000000000003</v>
+      </c>
+      <c r="K60" s="19">
+        <v>0.23799999999999999</v>
+      </c>
+      <c r="L60" s="19">
+        <v>0.27100000000000002</v>
+      </c>
+      <c r="M60" s="11">
+        <v>0.28199999999999997</v>
+      </c>
+      <c r="N60" s="5">
         <f t="shared" si="31"/>
-        <v>#DIV/0!</v>
+        <v>0.26840000000000003</v>
       </c>
       <c r="O60" s="9"/>
       <c r="P60" s="10"/>
@@ -5056,7 +5346,7 @@
         <v>#DIV/0!</v>
       </c>
       <c r="U60" s="15"/>
-      <c r="V60" s="19"/>
+      <c r="V60" s="22"/>
       <c r="W60" s="4" t="s">
         <v>6</v>
       </c>
@@ -5069,14 +5359,24 @@
         <f t="shared" si="33"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="AD60" s="9"/>
-      <c r="AE60" s="10"/>
-      <c r="AF60" s="10"/>
-      <c r="AG60" s="10"/>
-      <c r="AH60" s="11"/>
-      <c r="AI60" s="5" t="e">
+      <c r="AD60" s="9">
+        <v>920.3</v>
+      </c>
+      <c r="AE60" s="19">
+        <v>893.4</v>
+      </c>
+      <c r="AF60" s="19">
+        <v>1048</v>
+      </c>
+      <c r="AG60" s="19">
+        <v>922.2</v>
+      </c>
+      <c r="AH60" s="11">
+        <v>885.5</v>
+      </c>
+      <c r="AI60" s="5">
         <f t="shared" si="34"/>
-        <v>#DIV/0!</v>
+        <v>933.87999999999988</v>
       </c>
       <c r="AJ60" s="9"/>
       <c r="AK60" s="10"/>
@@ -5089,7 +5389,7 @@
       </c>
     </row>
     <row r="61" spans="1:41" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A61" s="19"/>
+      <c r="A61" s="22"/>
       <c r="B61" s="4" t="s">
         <v>7</v>
       </c>
@@ -5102,14 +5402,24 @@
         <f t="shared" si="30"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="I61" s="9"/>
-      <c r="J61" s="10"/>
-      <c r="K61" s="10"/>
-      <c r="L61" s="10"/>
-      <c r="M61" s="11"/>
-      <c r="N61" s="5" t="e">
+      <c r="I61" s="9">
+        <v>0.29399999999999998</v>
+      </c>
+      <c r="J61" s="19">
+        <v>0.28100000000000003</v>
+      </c>
+      <c r="K61" s="19">
+        <v>0.28000000000000003</v>
+      </c>
+      <c r="L61" s="19">
+        <v>0.30199999999999999</v>
+      </c>
+      <c r="M61" s="11">
+        <v>0.27900000000000003</v>
+      </c>
+      <c r="N61" s="5">
         <f t="shared" si="31"/>
-        <v>#DIV/0!</v>
+        <v>0.28720000000000001</v>
       </c>
       <c r="O61" s="9"/>
       <c r="P61" s="10"/>
@@ -5121,7 +5431,7 @@
         <v>#DIV/0!</v>
       </c>
       <c r="U61" s="15"/>
-      <c r="V61" s="19"/>
+      <c r="V61" s="22"/>
       <c r="W61" s="4" t="s">
         <v>7</v>
       </c>
@@ -5134,14 +5444,24 @@
         <f t="shared" si="33"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="AD61" s="9"/>
-      <c r="AE61" s="10"/>
-      <c r="AF61" s="10"/>
-      <c r="AG61" s="10"/>
-      <c r="AH61" s="11"/>
-      <c r="AI61" s="5" t="e">
+      <c r="AD61" s="9">
+        <v>1698</v>
+      </c>
+      <c r="AE61" s="19">
+        <v>1776</v>
+      </c>
+      <c r="AF61" s="19">
+        <v>1784</v>
+      </c>
+      <c r="AG61" s="19">
+        <v>1657</v>
+      </c>
+      <c r="AH61" s="11">
+        <v>1791</v>
+      </c>
+      <c r="AI61" s="5">
         <f t="shared" si="34"/>
-        <v>#DIV/0!</v>
+        <v>1741.2</v>
       </c>
       <c r="AJ61" s="9"/>
       <c r="AK61" s="10"/>
@@ -5154,7 +5474,7 @@
       </c>
     </row>
     <row r="62" spans="1:41" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A62" s="19"/>
+      <c r="A62" s="22"/>
       <c r="B62" s="4" t="s">
         <v>8</v>
       </c>
@@ -5167,14 +5487,24 @@
         <f t="shared" si="30"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="I62" s="9"/>
-      <c r="J62" s="10"/>
-      <c r="K62" s="10"/>
-      <c r="L62" s="10"/>
-      <c r="M62" s="11"/>
-      <c r="N62" s="5" t="e">
+      <c r="I62" s="9">
+        <v>0.31</v>
+      </c>
+      <c r="J62" s="19">
+        <v>0.317</v>
+      </c>
+      <c r="K62" s="19">
+        <v>0.309</v>
+      </c>
+      <c r="L62" s="19">
+        <v>0.312</v>
+      </c>
+      <c r="M62" s="11">
+        <v>0.29199999999999998</v>
+      </c>
+      <c r="N62" s="5">
         <f t="shared" si="31"/>
-        <v>#DIV/0!</v>
+        <v>0.308</v>
       </c>
       <c r="O62" s="9"/>
       <c r="P62" s="10"/>
@@ -5186,7 +5516,7 @@
         <v>#DIV/0!</v>
       </c>
       <c r="U62" s="15"/>
-      <c r="V62" s="19"/>
+      <c r="V62" s="22"/>
       <c r="W62" s="4" t="s">
         <v>8</v>
       </c>
@@ -5199,14 +5529,24 @@
         <f t="shared" si="33"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="AD62" s="9"/>
-      <c r="AE62" s="10"/>
-      <c r="AF62" s="10"/>
-      <c r="AG62" s="10"/>
-      <c r="AH62" s="11"/>
-      <c r="AI62" s="5" t="e">
+      <c r="AD62" s="9">
+        <v>2418</v>
+      </c>
+      <c r="AE62" s="19">
+        <v>2360</v>
+      </c>
+      <c r="AF62" s="19">
+        <v>2426</v>
+      </c>
+      <c r="AG62" s="19">
+        <v>2405</v>
+      </c>
+      <c r="AH62" s="11">
+        <v>2563</v>
+      </c>
+      <c r="AI62" s="5">
         <f t="shared" si="34"/>
-        <v>#DIV/0!</v>
+        <v>2434.4</v>
       </c>
       <c r="AJ62" s="9"/>
       <c r="AK62" s="10"/>
@@ -5219,7 +5559,7 @@
       </c>
     </row>
     <row r="63" spans="1:41" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A63" s="19"/>
+      <c r="A63" s="22"/>
       <c r="B63" s="4" t="s">
         <v>9</v>
       </c>
@@ -5232,14 +5572,24 @@
         <f t="shared" si="30"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="I63" s="12"/>
-      <c r="J63" s="13"/>
-      <c r="K63" s="13"/>
-      <c r="L63" s="13"/>
-      <c r="M63" s="14"/>
-      <c r="N63" s="5" t="e">
+      <c r="I63" s="12">
+        <v>0.33200000000000002</v>
+      </c>
+      <c r="J63" s="13">
+        <v>0.315</v>
+      </c>
+      <c r="K63" s="13">
+        <v>0.30099999999999999</v>
+      </c>
+      <c r="L63" s="13">
+        <v>0.32600000000000001</v>
+      </c>
+      <c r="M63" s="14">
+        <v>0.32300000000000001</v>
+      </c>
+      <c r="N63" s="5">
         <f t="shared" si="31"/>
-        <v>#DIV/0!</v>
+        <v>0.31940000000000002</v>
       </c>
       <c r="O63" s="12"/>
       <c r="P63" s="13"/>
@@ -5251,7 +5601,7 @@
         <v>#DIV/0!</v>
       </c>
       <c r="U63" s="15"/>
-      <c r="V63" s="19"/>
+      <c r="V63" s="22"/>
       <c r="W63" s="4" t="s">
         <v>9</v>
       </c>
@@ -5264,14 +5614,24 @@
         <f t="shared" si="33"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="AD63" s="12"/>
-      <c r="AE63" s="13"/>
-      <c r="AF63" s="13"/>
-      <c r="AG63" s="13"/>
-      <c r="AH63" s="14"/>
-      <c r="AI63" s="5" t="e">
+      <c r="AD63" s="12">
+        <v>3007</v>
+      </c>
+      <c r="AE63" s="13">
+        <v>3173</v>
+      </c>
+      <c r="AF63" s="13">
+        <v>3324</v>
+      </c>
+      <c r="AG63" s="13">
+        <v>3066</v>
+      </c>
+      <c r="AH63" s="14">
+        <v>3095</v>
+      </c>
+      <c r="AI63" s="5">
         <f t="shared" si="34"/>
-        <v>#DIV/0!</v>
+        <v>3133</v>
       </c>
       <c r="AJ63" s="12"/>
       <c r="AK63" s="13"/>
@@ -5327,7 +5687,7 @@
       <c r="AO64" s="15"/>
     </row>
     <row r="65" spans="1:41" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A65" s="19" t="s">
+      <c r="A65" s="22" t="s">
         <v>25</v>
       </c>
       <c r="B65" s="4" t="s">
@@ -5342,14 +5702,24 @@
         <f>AVERAGE(C65:G65)</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="I65" s="6"/>
-      <c r="J65" s="7"/>
-      <c r="K65" s="7"/>
-      <c r="L65" s="7"/>
-      <c r="M65" s="8"/>
-      <c r="N65" s="5" t="e">
+      <c r="I65" s="6">
+        <v>0.36099999999999999</v>
+      </c>
+      <c r="J65" s="7">
+        <v>0.28199999999999997</v>
+      </c>
+      <c r="K65" s="7">
+        <v>0.28399999999999997</v>
+      </c>
+      <c r="L65" s="7">
+        <v>0.29099999999999998</v>
+      </c>
+      <c r="M65" s="8">
+        <v>0.27900000000000003</v>
+      </c>
+      <c r="N65" s="5">
         <f>AVERAGE(I65:M65)</f>
-        <v>#DIV/0!</v>
+        <v>0.2994</v>
       </c>
       <c r="O65" s="6"/>
       <c r="P65" s="7"/>
@@ -5361,7 +5731,7 @@
         <v>#DIV/0!</v>
       </c>
       <c r="U65" s="15"/>
-      <c r="V65" s="19" t="s">
+      <c r="V65" s="22" t="s">
         <v>25</v>
       </c>
       <c r="W65" s="4" t="s">
@@ -5376,14 +5746,24 @@
         <f>AVERAGE(X65:AB65)</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="AD65" s="6"/>
-      <c r="AE65" s="7"/>
-      <c r="AF65" s="7"/>
-      <c r="AG65" s="7"/>
-      <c r="AH65" s="8"/>
-      <c r="AI65" s="5" t="e">
+      <c r="AD65" s="6">
+        <v>82.37</v>
+      </c>
+      <c r="AE65" s="7">
+        <v>105.4</v>
+      </c>
+      <c r="AF65" s="7">
+        <v>104.6</v>
+      </c>
+      <c r="AG65" s="7">
+        <v>102.2</v>
+      </c>
+      <c r="AH65" s="8">
+        <v>106.4</v>
+      </c>
+      <c r="AI65" s="5">
         <f>AVERAGE(AD65:AH65)</f>
-        <v>#DIV/0!</v>
+        <v>100.194</v>
       </c>
       <c r="AJ65" s="6"/>
       <c r="AK65" s="7"/>
@@ -5396,7 +5776,7 @@
       </c>
     </row>
     <row r="66" spans="1:41" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A66" s="19"/>
+      <c r="A66" s="22"/>
       <c r="B66" s="4" t="s">
         <v>2</v>
       </c>
@@ -5409,14 +5789,24 @@
         <f t="shared" ref="H66:H73" si="36">AVERAGE(C66:G66)</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="I66" s="9"/>
-      <c r="J66" s="10"/>
-      <c r="K66" s="10"/>
-      <c r="L66" s="10"/>
-      <c r="M66" s="11"/>
-      <c r="N66" s="5" t="e">
+      <c r="I66" s="9">
+        <v>0.91100000000000003</v>
+      </c>
+      <c r="J66" s="19">
+        <v>0.90300000000000002</v>
+      </c>
+      <c r="K66" s="19">
+        <v>0.89700000000000002</v>
+      </c>
+      <c r="L66" s="19">
+        <v>0.91</v>
+      </c>
+      <c r="M66" s="11">
+        <v>0.877</v>
+      </c>
+      <c r="N66" s="5">
         <f t="shared" ref="N66:N73" si="37">AVERAGE(I66:M66)</f>
-        <v>#DIV/0!</v>
+        <v>0.89960000000000007</v>
       </c>
       <c r="O66" s="9"/>
       <c r="P66" s="10"/>
@@ -5428,7 +5818,7 @@
         <v>#DIV/0!</v>
       </c>
       <c r="U66" s="15"/>
-      <c r="V66" s="19"/>
+      <c r="V66" s="22"/>
       <c r="W66" s="4" t="s">
         <v>2</v>
       </c>
@@ -5441,14 +5831,24 @@
         <f t="shared" ref="AC66:AC73" si="39">AVERAGE(X66:AB66)</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="AD66" s="9"/>
-      <c r="AE66" s="10"/>
-      <c r="AF66" s="10"/>
-      <c r="AG66" s="10"/>
-      <c r="AH66" s="11"/>
-      <c r="AI66" s="5" t="e">
+      <c r="AD66" s="9">
+        <v>6454</v>
+      </c>
+      <c r="AE66" s="19">
+        <v>6510</v>
+      </c>
+      <c r="AF66" s="19">
+        <v>6552</v>
+      </c>
+      <c r="AG66" s="19">
+        <v>6459</v>
+      </c>
+      <c r="AH66" s="11">
+        <v>6708</v>
+      </c>
+      <c r="AI66" s="5">
         <f t="shared" ref="AI66:AI73" si="40">AVERAGE(AD66:AH66)</f>
-        <v>#DIV/0!</v>
+        <v>6536.6</v>
       </c>
       <c r="AJ66" s="9"/>
       <c r="AK66" s="10"/>
@@ -5461,7 +5861,7 @@
       </c>
     </row>
     <row r="67" spans="1:41" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A67" s="19"/>
+      <c r="A67" s="22"/>
       <c r="B67" s="4" t="s">
         <v>3</v>
       </c>
@@ -5474,14 +5874,24 @@
         <f t="shared" si="36"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="I67" s="9"/>
-      <c r="J67" s="10"/>
-      <c r="K67" s="10"/>
-      <c r="L67" s="10"/>
-      <c r="M67" s="11"/>
-      <c r="N67" s="5" t="e">
+      <c r="I67" s="9">
+        <v>2.6139999999999999</v>
+      </c>
+      <c r="J67" s="19">
+        <v>2.5619999999999998</v>
+      </c>
+      <c r="K67" s="19">
+        <v>2.581</v>
+      </c>
+      <c r="L67" s="19">
+        <v>2.5350000000000001</v>
+      </c>
+      <c r="M67" s="11">
+        <v>2.5569999999999999</v>
+      </c>
+      <c r="N67" s="5">
         <f t="shared" si="37"/>
-        <v>#DIV/0!</v>
+        <v>2.5697999999999999</v>
       </c>
       <c r="O67" s="9"/>
       <c r="P67" s="10"/>
@@ -5493,7 +5903,7 @@
         <v>#DIV/0!</v>
       </c>
       <c r="U67" s="15"/>
-      <c r="V67" s="19"/>
+      <c r="V67" s="22"/>
       <c r="W67" s="4" t="s">
         <v>3</v>
       </c>
@@ -5506,14 +5916,24 @@
         <f t="shared" si="39"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="AD67" s="9"/>
-      <c r="AE67" s="10"/>
-      <c r="AF67" s="10"/>
-      <c r="AG67" s="10"/>
-      <c r="AH67" s="11"/>
-      <c r="AI67" s="5" t="e">
+      <c r="AD67" s="9">
+        <v>7982</v>
+      </c>
+      <c r="AE67" s="19">
+        <v>8146</v>
+      </c>
+      <c r="AF67" s="19">
+        <v>8086</v>
+      </c>
+      <c r="AG67" s="19">
+        <v>8232</v>
+      </c>
+      <c r="AH67" s="11">
+        <v>8162</v>
+      </c>
+      <c r="AI67" s="5">
         <f t="shared" si="40"/>
-        <v>#DIV/0!</v>
+        <v>8121.6</v>
       </c>
       <c r="AJ67" s="9"/>
       <c r="AK67" s="10"/>
@@ -5526,7 +5946,7 @@
       </c>
     </row>
     <row r="68" spans="1:41" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A68" s="19"/>
+      <c r="A68" s="22"/>
       <c r="B68" s="4" t="s">
         <v>4</v>
       </c>
@@ -5539,14 +5959,24 @@
         <f t="shared" si="36"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="I68" s="9"/>
-      <c r="J68" s="10"/>
-      <c r="K68" s="10"/>
-      <c r="L68" s="10"/>
-      <c r="M68" s="11"/>
-      <c r="N68" s="5" t="e">
+      <c r="I68" s="9">
+        <v>7.4690000000000003</v>
+      </c>
+      <c r="J68" s="19">
+        <v>7.7140000000000004</v>
+      </c>
+      <c r="K68" s="19">
+        <v>7.6050000000000004</v>
+      </c>
+      <c r="L68" s="19">
+        <v>7.4329999999999998</v>
+      </c>
+      <c r="M68" s="11">
+        <v>7.524</v>
+      </c>
+      <c r="N68" s="5">
         <f t="shared" si="37"/>
-        <v>#DIV/0!</v>
+        <v>7.5489999999999995</v>
       </c>
       <c r="O68" s="9"/>
       <c r="P68" s="10"/>
@@ -5558,7 +5988,7 @@
         <v>#DIV/0!</v>
       </c>
       <c r="U68" s="15"/>
-      <c r="V68" s="19"/>
+      <c r="V68" s="22"/>
       <c r="W68" s="4" t="s">
         <v>4</v>
       </c>
@@ -5571,14 +6001,24 @@
         <f t="shared" si="39"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="AD68" s="9"/>
-      <c r="AE68" s="10"/>
-      <c r="AF68" s="10"/>
-      <c r="AG68" s="10"/>
-      <c r="AH68" s="11"/>
-      <c r="AI68" s="5" t="e">
+      <c r="AD68" s="9">
+        <v>11090</v>
+      </c>
+      <c r="AE68" s="19">
+        <v>10730</v>
+      </c>
+      <c r="AF68" s="19">
+        <v>10890</v>
+      </c>
+      <c r="AG68" s="19">
+        <v>11140</v>
+      </c>
+      <c r="AH68" s="11">
+        <v>11010</v>
+      </c>
+      <c r="AI68" s="5">
         <f t="shared" si="40"/>
-        <v>#DIV/0!</v>
+        <v>10972</v>
       </c>
       <c r="AJ68" s="9"/>
       <c r="AK68" s="10"/>
@@ -5591,7 +6031,7 @@
       </c>
     </row>
     <row r="69" spans="1:41" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A69" s="19"/>
+      <c r="A69" s="22"/>
       <c r="B69" s="4" t="s">
         <v>5</v>
       </c>
@@ -5604,14 +6044,24 @@
         <f t="shared" si="36"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="I69" s="9"/>
-      <c r="J69" s="10"/>
-      <c r="K69" s="10"/>
-      <c r="L69" s="10"/>
-      <c r="M69" s="11"/>
-      <c r="N69" s="5" t="e">
+      <c r="I69" s="9">
+        <v>13.439</v>
+      </c>
+      <c r="J69" s="19">
+        <v>13.247</v>
+      </c>
+      <c r="K69" s="19">
+        <v>13.263999999999999</v>
+      </c>
+      <c r="L69" s="19">
+        <v>12.935</v>
+      </c>
+      <c r="M69" s="11">
+        <v>13.045999999999999</v>
+      </c>
+      <c r="N69" s="5">
         <f t="shared" si="37"/>
-        <v>#DIV/0!</v>
+        <v>13.186200000000003</v>
       </c>
       <c r="O69" s="9"/>
       <c r="P69" s="10"/>
@@ -5623,7 +6073,7 @@
         <v>#DIV/0!</v>
       </c>
       <c r="U69" s="15"/>
-      <c r="V69" s="19"/>
+      <c r="V69" s="22"/>
       <c r="W69" s="4" t="s">
         <v>5</v>
       </c>
@@ -5636,14 +6086,24 @@
         <f t="shared" si="39"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="AD69" s="9"/>
-      <c r="AE69" s="10"/>
-      <c r="AF69" s="10"/>
-      <c r="AG69" s="10"/>
-      <c r="AH69" s="11"/>
-      <c r="AI69" s="5" t="e">
+      <c r="AD69" s="9">
+        <v>12010</v>
+      </c>
+      <c r="AE69" s="19">
+        <v>12190</v>
+      </c>
+      <c r="AF69" s="19">
+        <v>12170</v>
+      </c>
+      <c r="AG69" s="19">
+        <v>12480</v>
+      </c>
+      <c r="AH69" s="11">
+        <v>12370</v>
+      </c>
+      <c r="AI69" s="5">
         <f t="shared" si="40"/>
-        <v>#DIV/0!</v>
+        <v>12244</v>
       </c>
       <c r="AJ69" s="9"/>
       <c r="AK69" s="10"/>
@@ -5656,7 +6116,7 @@
       </c>
     </row>
     <row r="70" spans="1:41" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A70" s="19"/>
+      <c r="A70" s="22"/>
       <c r="B70" s="4" t="s">
         <v>6</v>
       </c>
@@ -5669,14 +6129,24 @@
         <f t="shared" si="36"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="I70" s="9"/>
-      <c r="J70" s="10"/>
-      <c r="K70" s="10"/>
-      <c r="L70" s="10"/>
-      <c r="M70" s="11"/>
-      <c r="N70" s="5" t="e">
+      <c r="I70" s="9">
+        <v>0.26600000000000001</v>
+      </c>
+      <c r="J70" s="19">
+        <v>0.27700000000000002</v>
+      </c>
+      <c r="K70" s="19">
+        <v>0.27400000000000002</v>
+      </c>
+      <c r="L70" s="19">
+        <v>0.26700000000000002</v>
+      </c>
+      <c r="M70" s="11">
+        <v>0.26600000000000001</v>
+      </c>
+      <c r="N70" s="5">
         <f t="shared" si="37"/>
-        <v>#DIV/0!</v>
+        <v>0.27</v>
       </c>
       <c r="O70" s="9"/>
       <c r="P70" s="10"/>
@@ -5688,7 +6158,7 @@
         <v>#DIV/0!</v>
       </c>
       <c r="U70" s="15"/>
-      <c r="V70" s="19"/>
+      <c r="V70" s="22"/>
       <c r="W70" s="4" t="s">
         <v>6</v>
       </c>
@@ -5701,14 +6171,24 @@
         <f t="shared" si="39"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="AD70" s="9"/>
-      <c r="AE70" s="10"/>
-      <c r="AF70" s="10"/>
-      <c r="AG70" s="10"/>
-      <c r="AH70" s="11"/>
-      <c r="AI70" s="5" t="e">
+      <c r="AD70" s="9">
+        <v>940.5</v>
+      </c>
+      <c r="AE70" s="19">
+        <v>901.2</v>
+      </c>
+      <c r="AF70" s="19">
+        <v>912.1</v>
+      </c>
+      <c r="AG70" s="19">
+        <v>936.5</v>
+      </c>
+      <c r="AH70" s="11">
+        <v>940.1</v>
+      </c>
+      <c r="AI70" s="5">
         <f t="shared" si="40"/>
-        <v>#DIV/0!</v>
+        <v>926.08000000000015</v>
       </c>
       <c r="AJ70" s="9"/>
       <c r="AK70" s="10"/>
@@ -5721,7 +6201,7 @@
       </c>
     </row>
     <row r="71" spans="1:41" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A71" s="19"/>
+      <c r="A71" s="22"/>
       <c r="B71" s="4" t="s">
         <v>7</v>
       </c>
@@ -5734,14 +6214,24 @@
         <f t="shared" si="36"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="I71" s="9"/>
-      <c r="J71" s="10"/>
-      <c r="K71" s="10"/>
-      <c r="L71" s="10"/>
-      <c r="M71" s="11"/>
-      <c r="N71" s="5" t="e">
+      <c r="I71" s="9">
+        <v>0.27700000000000002</v>
+      </c>
+      <c r="J71" s="19">
+        <v>0.29199999999999998</v>
+      </c>
+      <c r="K71" s="19">
+        <v>0.27900000000000003</v>
+      </c>
+      <c r="L71" s="19">
+        <v>0.29299999999999998</v>
+      </c>
+      <c r="M71" s="11">
+        <v>0.29299999999999998</v>
+      </c>
+      <c r="N71" s="5">
         <f t="shared" si="37"/>
-        <v>#DIV/0!</v>
+        <v>0.2868</v>
       </c>
       <c r="O71" s="9"/>
       <c r="P71" s="10"/>
@@ -5753,7 +6243,7 @@
         <v>#DIV/0!</v>
       </c>
       <c r="U71" s="15"/>
-      <c r="V71" s="19"/>
+      <c r="V71" s="22"/>
       <c r="W71" s="4" t="s">
         <v>7</v>
       </c>
@@ -5766,14 +6256,24 @@
         <f t="shared" si="39"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="AD71" s="9"/>
-      <c r="AE71" s="10"/>
-      <c r="AF71" s="10"/>
-      <c r="AG71" s="10"/>
-      <c r="AH71" s="11"/>
-      <c r="AI71" s="5" t="e">
+      <c r="AD71" s="9">
+        <v>1803</v>
+      </c>
+      <c r="AE71" s="19">
+        <v>1712</v>
+      </c>
+      <c r="AF71" s="19">
+        <v>1791</v>
+      </c>
+      <c r="AG71" s="19">
+        <v>1705</v>
+      </c>
+      <c r="AH71" s="11">
+        <v>1707</v>
+      </c>
+      <c r="AI71" s="5">
         <f t="shared" si="40"/>
-        <v>#DIV/0!</v>
+        <v>1743.6</v>
       </c>
       <c r="AJ71" s="9"/>
       <c r="AK71" s="10"/>
@@ -5786,7 +6286,7 @@
       </c>
     </row>
     <row r="72" spans="1:41" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A72" s="19"/>
+      <c r="A72" s="22"/>
       <c r="B72" s="4" t="s">
         <v>8</v>
       </c>
@@ -5799,14 +6299,24 @@
         <f t="shared" si="36"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="I72" s="9"/>
-      <c r="J72" s="10"/>
-      <c r="K72" s="10"/>
-      <c r="L72" s="10"/>
-      <c r="M72" s="11"/>
-      <c r="N72" s="5" t="e">
+      <c r="I72" s="9">
+        <v>0.28799999999999998</v>
+      </c>
+      <c r="J72" s="19">
+        <v>0.30099999999999999</v>
+      </c>
+      <c r="K72" s="19">
+        <v>0.31</v>
+      </c>
+      <c r="L72" s="19">
+        <v>0.30199999999999999</v>
+      </c>
+      <c r="M72" s="11">
+        <v>0.30299999999999999</v>
+      </c>
+      <c r="N72" s="5">
         <f t="shared" si="37"/>
-        <v>#DIV/0!</v>
+        <v>0.30080000000000001</v>
       </c>
       <c r="O72" s="9"/>
       <c r="P72" s="10"/>
@@ -5818,7 +6328,7 @@
         <v>#DIV/0!</v>
       </c>
       <c r="U72" s="15"/>
-      <c r="V72" s="19"/>
+      <c r="V72" s="22"/>
       <c r="W72" s="4" t="s">
         <v>8</v>
       </c>
@@ -5831,14 +6341,24 @@
         <f t="shared" si="39"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="AD72" s="9"/>
-      <c r="AE72" s="10"/>
-      <c r="AF72" s="10"/>
-      <c r="AG72" s="10"/>
-      <c r="AH72" s="11"/>
-      <c r="AI72" s="5" t="e">
+      <c r="AD72" s="9">
+        <v>2604</v>
+      </c>
+      <c r="AE72" s="19">
+        <v>2488</v>
+      </c>
+      <c r="AF72" s="19">
+        <v>2416</v>
+      </c>
+      <c r="AG72" s="19">
+        <v>2484</v>
+      </c>
+      <c r="AH72" s="11">
+        <v>2469</v>
+      </c>
+      <c r="AI72" s="5">
         <f t="shared" si="40"/>
-        <v>#DIV/0!</v>
+        <v>2492.1999999999998</v>
       </c>
       <c r="AJ72" s="9"/>
       <c r="AK72" s="10"/>
@@ -5851,7 +6371,7 @@
       </c>
     </row>
     <row r="73" spans="1:41" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A73" s="19"/>
+      <c r="A73" s="22"/>
       <c r="B73" s="4" t="s">
         <v>9</v>
       </c>
@@ -5864,14 +6384,24 @@
         <f t="shared" si="36"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="I73" s="12"/>
-      <c r="J73" s="13"/>
-      <c r="K73" s="13"/>
-      <c r="L73" s="13"/>
-      <c r="M73" s="14"/>
-      <c r="N73" s="5" t="e">
+      <c r="I73" s="12">
+        <v>0.318</v>
+      </c>
+      <c r="J73" s="13">
+        <v>0.32700000000000001</v>
+      </c>
+      <c r="K73" s="13">
+        <v>0.32900000000000001</v>
+      </c>
+      <c r="L73" s="13">
+        <v>0.32400000000000001</v>
+      </c>
+      <c r="M73" s="14">
+        <v>0.32</v>
+      </c>
+      <c r="N73" s="5">
         <f t="shared" si="37"/>
-        <v>#DIV/0!</v>
+        <v>0.3236</v>
       </c>
       <c r="O73" s="12"/>
       <c r="P73" s="13"/>
@@ -5883,7 +6413,7 @@
         <v>#DIV/0!</v>
       </c>
       <c r="U73" s="15"/>
-      <c r="V73" s="19"/>
+      <c r="V73" s="22"/>
       <c r="W73" s="4" t="s">
         <v>9</v>
       </c>
@@ -5896,14 +6426,24 @@
         <f t="shared" si="39"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="AD73" s="12"/>
-      <c r="AE73" s="13"/>
-      <c r="AF73" s="13"/>
-      <c r="AG73" s="13"/>
-      <c r="AH73" s="14"/>
-      <c r="AI73" s="5" t="e">
+      <c r="AD73" s="12">
+        <v>3141</v>
+      </c>
+      <c r="AE73" s="13">
+        <v>3057</v>
+      </c>
+      <c r="AF73" s="13">
+        <v>3034</v>
+      </c>
+      <c r="AG73" s="13">
+        <v>3079</v>
+      </c>
+      <c r="AH73" s="14">
+        <v>3121</v>
+      </c>
+      <c r="AI73" s="5">
         <f t="shared" si="40"/>
-        <v>#DIV/0!</v>
+        <v>3086.4</v>
       </c>
       <c r="AJ73" s="12"/>
       <c r="AK73" s="13"/>
@@ -5959,7 +6499,7 @@
       <c r="AO74" s="15"/>
     </row>
     <row r="75" spans="1:41" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A75" s="19" t="s">
+      <c r="A75" s="22" t="s">
         <v>26</v>
       </c>
       <c r="B75" s="4" t="s">
@@ -5974,14 +6514,24 @@
         <f>AVERAGE(C75:G75)</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="I75" s="6"/>
-      <c r="J75" s="7"/>
-      <c r="K75" s="7"/>
-      <c r="L75" s="7"/>
-      <c r="M75" s="8"/>
-      <c r="N75" s="5" t="e">
+      <c r="I75" s="6">
+        <v>0.374</v>
+      </c>
+      <c r="J75" s="7">
+        <v>0.27800000000000002</v>
+      </c>
+      <c r="K75" s="7">
+        <v>0.29699999999999999</v>
+      </c>
+      <c r="L75" s="7">
+        <v>0.28799999999999998</v>
+      </c>
+      <c r="M75" s="8">
+        <v>0.28599999999999998</v>
+      </c>
+      <c r="N75" s="5">
         <f>AVERAGE(I75:M75)</f>
-        <v>#DIV/0!</v>
+        <v>0.30460000000000004</v>
       </c>
       <c r="O75" s="6"/>
       <c r="P75" s="7"/>
@@ -5993,7 +6543,7 @@
         <v>#DIV/0!</v>
       </c>
       <c r="U75" s="15"/>
-      <c r="V75" s="19" t="s">
+      <c r="V75" s="22" t="s">
         <v>26</v>
       </c>
       <c r="W75" s="4" t="s">
@@ -6008,14 +6558,24 @@
         <f>AVERAGE(X75:AB75)</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="AD75" s="6"/>
-      <c r="AE75" s="7"/>
-      <c r="AF75" s="7"/>
-      <c r="AG75" s="7"/>
-      <c r="AH75" s="8"/>
-      <c r="AI75" s="5" t="e">
+      <c r="AD75" s="6">
+        <v>79.42</v>
+      </c>
+      <c r="AE75" s="7">
+        <v>106.9</v>
+      </c>
+      <c r="AF75" s="7">
+        <v>99.9</v>
+      </c>
+      <c r="AG75" s="7">
+        <v>103.1</v>
+      </c>
+      <c r="AH75" s="8">
+        <v>13.7</v>
+      </c>
+      <c r="AI75" s="5">
         <f>AVERAGE(AD75:AH75)</f>
-        <v>#DIV/0!</v>
+        <v>80.604000000000013</v>
       </c>
       <c r="AJ75" s="6"/>
       <c r="AK75" s="7"/>
@@ -6028,7 +6588,7 @@
       </c>
     </row>
     <row r="76" spans="1:41" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A76" s="19"/>
+      <c r="A76" s="22"/>
       <c r="B76" s="4" t="s">
         <v>2</v>
       </c>
@@ -6041,14 +6601,24 @@
         <f t="shared" ref="H76:H83" si="42">AVERAGE(C76:G76)</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="I76" s="9"/>
-      <c r="J76" s="10"/>
-      <c r="K76" s="10"/>
-      <c r="L76" s="10"/>
-      <c r="M76" s="11"/>
-      <c r="N76" s="5" t="e">
+      <c r="I76" s="9">
+        <v>0.94099999999999995</v>
+      </c>
+      <c r="J76" s="19">
+        <v>0.92</v>
+      </c>
+      <c r="K76" s="19">
+        <v>0.88300000000000001</v>
+      </c>
+      <c r="L76" s="19">
+        <v>0.90600000000000003</v>
+      </c>
+      <c r="M76" s="11">
+        <v>0.88100000000000001</v>
+      </c>
+      <c r="N76" s="5">
         <f t="shared" ref="N76:N83" si="43">AVERAGE(I76:M76)</f>
-        <v>#DIV/0!</v>
+        <v>0.90619999999999989</v>
       </c>
       <c r="O76" s="9"/>
       <c r="P76" s="10"/>
@@ -6060,7 +6630,7 @@
         <v>#DIV/0!</v>
       </c>
       <c r="U76" s="15"/>
-      <c r="V76" s="19"/>
+      <c r="V76" s="22"/>
       <c r="W76" s="4" t="s">
         <v>2</v>
       </c>
@@ -6073,14 +6643,24 @@
         <f t="shared" ref="AC76:AC83" si="45">AVERAGE(X76:AB76)</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="AD76" s="9"/>
-      <c r="AE76" s="10"/>
-      <c r="AF76" s="10"/>
-      <c r="AG76" s="10"/>
-      <c r="AH76" s="11"/>
-      <c r="AI76" s="5" t="e">
+      <c r="AD76" s="9">
+        <v>6252</v>
+      </c>
+      <c r="AE76" s="19">
+        <v>6392</v>
+      </c>
+      <c r="AF76" s="19">
+        <v>6663</v>
+      </c>
+      <c r="AG76" s="19">
+        <v>6488</v>
+      </c>
+      <c r="AH76" s="11">
+        <v>6673</v>
+      </c>
+      <c r="AI76" s="5">
         <f t="shared" ref="AI76:AI83" si="46">AVERAGE(AD76:AH76)</f>
-        <v>#DIV/0!</v>
+        <v>6493.6</v>
       </c>
       <c r="AJ76" s="9"/>
       <c r="AK76" s="10"/>
@@ -6093,7 +6673,7 @@
       </c>
     </row>
     <row r="77" spans="1:41" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A77" s="19"/>
+      <c r="A77" s="22"/>
       <c r="B77" s="4" t="s">
         <v>3</v>
       </c>
@@ -6106,14 +6686,24 @@
         <f t="shared" si="42"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="I77" s="9"/>
-      <c r="J77" s="10"/>
-      <c r="K77" s="10"/>
-      <c r="L77" s="10"/>
-      <c r="M77" s="11"/>
-      <c r="N77" s="5" t="e">
+      <c r="I77" s="9">
+        <v>2.7669999999999999</v>
+      </c>
+      <c r="J77" s="19">
+        <v>2.7519999999999998</v>
+      </c>
+      <c r="K77" s="19">
+        <v>2.7839999999999998</v>
+      </c>
+      <c r="L77" s="19">
+        <v>2.7919999999999998</v>
+      </c>
+      <c r="M77" s="11">
+        <v>2.7589999999999999</v>
+      </c>
+      <c r="N77" s="5">
         <f t="shared" si="43"/>
-        <v>#DIV/0!</v>
+        <v>2.7708000000000004</v>
       </c>
       <c r="O77" s="9"/>
       <c r="P77" s="10"/>
@@ -6125,7 +6715,7 @@
         <v>#DIV/0!</v>
       </c>
       <c r="U77" s="15"/>
-      <c r="V77" s="19"/>
+      <c r="V77" s="22"/>
       <c r="W77" s="4" t="s">
         <v>3</v>
       </c>
@@ -6138,14 +6728,24 @@
         <f t="shared" si="45"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="AD77" s="9"/>
-      <c r="AE77" s="10"/>
-      <c r="AF77" s="10"/>
-      <c r="AG77" s="10"/>
-      <c r="AH77" s="11"/>
-      <c r="AI77" s="5" t="e">
+      <c r="AD77" s="9">
+        <v>7541</v>
+      </c>
+      <c r="AE77" s="19">
+        <v>7582</v>
+      </c>
+      <c r="AF77" s="19">
+        <v>7494</v>
+      </c>
+      <c r="AG77" s="19">
+        <v>7474</v>
+      </c>
+      <c r="AH77" s="11">
+        <v>7564</v>
+      </c>
+      <c r="AI77" s="5">
         <f t="shared" si="46"/>
-        <v>#DIV/0!</v>
+        <v>7531</v>
       </c>
       <c r="AJ77" s="9"/>
       <c r="AK77" s="10"/>
@@ -6158,7 +6758,7 @@
       </c>
     </row>
     <row r="78" spans="1:41" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A78" s="19"/>
+      <c r="A78" s="22"/>
       <c r="B78" s="4" t="s">
         <v>4</v>
       </c>
@@ -6171,14 +6771,24 @@
         <f t="shared" si="42"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="I78" s="9"/>
-      <c r="J78" s="10"/>
-      <c r="K78" s="10"/>
-      <c r="L78" s="10"/>
-      <c r="M78" s="11"/>
-      <c r="N78" s="5" t="e">
+      <c r="I78" s="9">
+        <v>8.1010000000000009</v>
+      </c>
+      <c r="J78" s="19">
+        <v>8.0890000000000004</v>
+      </c>
+      <c r="K78" s="19">
+        <v>8.2650000000000006</v>
+      </c>
+      <c r="L78" s="19">
+        <v>8.1780000000000008</v>
+      </c>
+      <c r="M78" s="11">
+        <v>8.2710000000000008</v>
+      </c>
+      <c r="N78" s="5">
         <f t="shared" si="43"/>
-        <v>#DIV/0!</v>
+        <v>8.1808000000000014</v>
       </c>
       <c r="O78" s="9"/>
       <c r="P78" s="10"/>
@@ -6190,7 +6800,7 @@
         <v>#DIV/0!</v>
       </c>
       <c r="U78" s="15"/>
-      <c r="V78" s="19"/>
+      <c r="V78" s="22"/>
       <c r="W78" s="4" t="s">
         <v>4</v>
       </c>
@@ -6203,14 +6813,24 @@
         <f t="shared" si="45"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="AD78" s="9"/>
-      <c r="AE78" s="10"/>
-      <c r="AF78" s="10"/>
-      <c r="AG78" s="10"/>
-      <c r="AH78" s="11"/>
-      <c r="AI78" s="5" t="e">
+      <c r="AD78" s="9">
+        <v>10220</v>
+      </c>
+      <c r="AE78" s="19">
+        <v>10240</v>
+      </c>
+      <c r="AF78" s="19">
+        <v>10020</v>
+      </c>
+      <c r="AG78" s="19">
+        <v>10120</v>
+      </c>
+      <c r="AH78" s="11">
+        <v>10010</v>
+      </c>
+      <c r="AI78" s="5">
         <f t="shared" si="46"/>
-        <v>#DIV/0!</v>
+        <v>10122</v>
       </c>
       <c r="AJ78" s="9"/>
       <c r="AK78" s="10"/>
@@ -6223,7 +6843,7 @@
       </c>
     </row>
     <row r="79" spans="1:41" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A79" s="19"/>
+      <c r="A79" s="22"/>
       <c r="B79" s="4" t="s">
         <v>5</v>
       </c>
@@ -6236,14 +6856,24 @@
         <f t="shared" si="42"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="I79" s="9"/>
-      <c r="J79" s="10"/>
-      <c r="K79" s="10"/>
-      <c r="L79" s="10"/>
-      <c r="M79" s="11"/>
-      <c r="N79" s="5" t="e">
+      <c r="I79" s="9">
+        <v>14.422000000000001</v>
+      </c>
+      <c r="J79" s="19">
+        <v>14.275</v>
+      </c>
+      <c r="K79" s="19">
+        <v>14.256</v>
+      </c>
+      <c r="L79" s="19">
+        <v>14.205</v>
+      </c>
+      <c r="M79" s="11">
+        <v>14.253</v>
+      </c>
+      <c r="N79" s="5">
         <f t="shared" si="43"/>
-        <v>#DIV/0!</v>
+        <v>14.2822</v>
       </c>
       <c r="O79" s="9"/>
       <c r="P79" s="10"/>
@@ -6255,7 +6885,7 @@
         <v>#DIV/0!</v>
       </c>
       <c r="U79" s="15"/>
-      <c r="V79" s="19"/>
+      <c r="V79" s="22"/>
       <c r="W79" s="4" t="s">
         <v>5</v>
       </c>
@@ -6268,14 +6898,24 @@
         <f t="shared" si="45"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="AD79" s="9"/>
-      <c r="AE79" s="10"/>
-      <c r="AF79" s="10"/>
-      <c r="AG79" s="10"/>
-      <c r="AH79" s="11"/>
-      <c r="AI79" s="5" t="e">
+      <c r="AD79" s="9">
+        <v>11190</v>
+      </c>
+      <c r="AE79" s="19">
+        <v>11310</v>
+      </c>
+      <c r="AF79" s="19">
+        <v>11320</v>
+      </c>
+      <c r="AG79" s="19">
+        <v>11370</v>
+      </c>
+      <c r="AH79" s="11">
+        <v>11330</v>
+      </c>
+      <c r="AI79" s="5">
         <f t="shared" si="46"/>
-        <v>#DIV/0!</v>
+        <v>11304</v>
       </c>
       <c r="AJ79" s="9"/>
       <c r="AK79" s="10"/>
@@ -6288,7 +6928,7 @@
       </c>
     </row>
     <row r="80" spans="1:41" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A80" s="19"/>
+      <c r="A80" s="22"/>
       <c r="B80" s="4" t="s">
         <v>6</v>
       </c>
@@ -6301,14 +6941,24 @@
         <f t="shared" si="42"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="I80" s="9"/>
-      <c r="J80" s="10"/>
-      <c r="K80" s="10"/>
-      <c r="L80" s="10"/>
-      <c r="M80" s="11"/>
-      <c r="N80" s="5" t="e">
+      <c r="I80" s="9">
+        <v>0.27200000000000002</v>
+      </c>
+      <c r="J80" s="19">
+        <v>0.27900000000000003</v>
+      </c>
+      <c r="K80" s="19">
+        <v>0.254</v>
+      </c>
+      <c r="L80" s="19">
+        <v>0.28000000000000003</v>
+      </c>
+      <c r="M80" s="11">
+        <v>0.27300000000000002</v>
+      </c>
+      <c r="N80" s="5">
         <f t="shared" si="43"/>
-        <v>#DIV/0!</v>
+        <v>0.27160000000000001</v>
       </c>
       <c r="O80" s="9"/>
       <c r="P80" s="10"/>
@@ -6320,7 +6970,7 @@
         <v>#DIV/0!</v>
       </c>
       <c r="U80" s="15"/>
-      <c r="V80" s="19"/>
+      <c r="V80" s="22"/>
       <c r="W80" s="4" t="s">
         <v>6</v>
       </c>
@@ -6333,14 +6983,24 @@
         <f t="shared" si="45"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="AD80" s="9"/>
-      <c r="AE80" s="10"/>
-      <c r="AF80" s="10"/>
-      <c r="AG80" s="10"/>
-      <c r="AH80" s="11"/>
-      <c r="AI80" s="5" t="e">
+      <c r="AD80" s="9">
+        <v>918.9</v>
+      </c>
+      <c r="AE80" s="19">
+        <v>894.8</v>
+      </c>
+      <c r="AF80" s="19">
+        <v>983.1</v>
+      </c>
+      <c r="AG80" s="19">
+        <v>893.7</v>
+      </c>
+      <c r="AH80" s="11">
+        <v>913.4</v>
+      </c>
+      <c r="AI80" s="5">
         <f t="shared" si="46"/>
-        <v>#DIV/0!</v>
+        <v>920.78</v>
       </c>
       <c r="AJ80" s="9"/>
       <c r="AK80" s="10"/>
@@ -6353,7 +7013,7 @@
       </c>
     </row>
     <row r="81" spans="1:41" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A81" s="19"/>
+      <c r="A81" s="22"/>
       <c r="B81" s="4" t="s">
         <v>7</v>
       </c>
@@ -6366,14 +7026,24 @@
         <f t="shared" si="42"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="I81" s="9"/>
-      <c r="J81" s="10"/>
-      <c r="K81" s="10"/>
-      <c r="L81" s="10"/>
-      <c r="M81" s="11"/>
-      <c r="N81" s="5" t="e">
+      <c r="I81" s="9">
+        <v>0.27300000000000002</v>
+      </c>
+      <c r="J81" s="19">
+        <v>0.29299999999999998</v>
+      </c>
+      <c r="K81" s="19">
+        <v>0.29399999999999998</v>
+      </c>
+      <c r="L81" s="19">
+        <v>0.28899999999999998</v>
+      </c>
+      <c r="M81" s="11">
+        <v>0.29099999999999998</v>
+      </c>
+      <c r="N81" s="5">
         <f t="shared" si="43"/>
-        <v>#DIV/0!</v>
+        <v>0.28799999999999998</v>
       </c>
       <c r="O81" s="9"/>
       <c r="P81" s="10"/>
@@ -6385,7 +7055,7 @@
         <v>#DIV/0!</v>
       </c>
       <c r="U81" s="15"/>
-      <c r="V81" s="19"/>
+      <c r="V81" s="22"/>
       <c r="W81" s="4" t="s">
         <v>7</v>
       </c>
@@ -6398,14 +7068,24 @@
         <f t="shared" si="45"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="AD81" s="9"/>
-      <c r="AE81" s="10"/>
-      <c r="AF81" s="10"/>
-      <c r="AG81" s="10"/>
-      <c r="AH81" s="11"/>
-      <c r="AI81" s="5" t="e">
+      <c r="AD81" s="9">
+        <v>1828</v>
+      </c>
+      <c r="AE81" s="19">
+        <v>1707</v>
+      </c>
+      <c r="AF81" s="19">
+        <v>1698</v>
+      </c>
+      <c r="AG81" s="19">
+        <v>1730</v>
+      </c>
+      <c r="AH81" s="11">
+        <v>1714</v>
+      </c>
+      <c r="AI81" s="5">
         <f t="shared" si="46"/>
-        <v>#DIV/0!</v>
+        <v>1735.4</v>
       </c>
       <c r="AJ81" s="9"/>
       <c r="AK81" s="10"/>
@@ -6418,7 +7098,7 @@
       </c>
     </row>
     <row r="82" spans="1:41" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A82" s="19"/>
+      <c r="A82" s="22"/>
       <c r="B82" s="4" t="s">
         <v>8</v>
       </c>
@@ -6431,14 +7111,24 @@
         <f t="shared" si="42"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="I82" s="9"/>
-      <c r="J82" s="10"/>
-      <c r="K82" s="10"/>
-      <c r="L82" s="10"/>
-      <c r="M82" s="11"/>
-      <c r="N82" s="5" t="e">
+      <c r="I82" s="9">
+        <v>0.28499999999999998</v>
+      </c>
+      <c r="J82" s="19">
+        <v>0.27300000000000002</v>
+      </c>
+      <c r="K82" s="19">
+        <v>0.311</v>
+      </c>
+      <c r="L82" s="19">
+        <v>0.30499999999999999</v>
+      </c>
+      <c r="M82" s="11">
+        <v>0.30299999999999999</v>
+      </c>
+      <c r="N82" s="5">
         <f t="shared" si="43"/>
-        <v>#DIV/0!</v>
+        <v>0.2954</v>
       </c>
       <c r="O82" s="9"/>
       <c r="P82" s="10"/>
@@ -6450,7 +7140,7 @@
         <v>#DIV/0!</v>
       </c>
       <c r="U82" s="15"/>
-      <c r="V82" s="19"/>
+      <c r="V82" s="22"/>
       <c r="W82" s="4" t="s">
         <v>8</v>
       </c>
@@ -6463,14 +7153,24 @@
         <f t="shared" si="45"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="AD82" s="9"/>
-      <c r="AE82" s="10"/>
-      <c r="AF82" s="10"/>
-      <c r="AG82" s="10"/>
-      <c r="AH82" s="11"/>
-      <c r="AI82" s="5" t="e">
+      <c r="AD82" s="9">
+        <v>2630</v>
+      </c>
+      <c r="AE82" s="19">
+        <v>2741</v>
+      </c>
+      <c r="AF82" s="19">
+        <v>2406</v>
+      </c>
+      <c r="AG82" s="19">
+        <v>2459</v>
+      </c>
+      <c r="AH82" s="11">
+        <v>2473</v>
+      </c>
+      <c r="AI82" s="5">
         <f t="shared" si="46"/>
-        <v>#DIV/0!</v>
+        <v>2541.8000000000002</v>
       </c>
       <c r="AJ82" s="9"/>
       <c r="AK82" s="10"/>
@@ -6483,7 +7183,7 @@
       </c>
     </row>
     <row r="83" spans="1:41" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A83" s="19"/>
+      <c r="A83" s="22"/>
       <c r="B83" s="4" t="s">
         <v>9</v>
       </c>
@@ -6496,14 +7196,24 @@
         <f t="shared" si="42"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="I83" s="12"/>
-      <c r="J83" s="13"/>
-      <c r="K83" s="13"/>
-      <c r="L83" s="13"/>
-      <c r="M83" s="14"/>
-      <c r="N83" s="5" t="e">
+      <c r="I83" s="12">
+        <v>0.32600000000000001</v>
+      </c>
+      <c r="J83" s="13">
+        <v>0.30499999999999999</v>
+      </c>
+      <c r="K83" s="13">
+        <v>0.32200000000000001</v>
+      </c>
+      <c r="L83" s="13">
+        <v>0.30499999999999999</v>
+      </c>
+      <c r="M83" s="14">
+        <v>0.31900000000000001</v>
+      </c>
+      <c r="N83" s="5">
         <f t="shared" si="43"/>
-        <v>#DIV/0!</v>
+        <v>0.31540000000000001</v>
       </c>
       <c r="O83" s="12"/>
       <c r="P83" s="13"/>
@@ -6515,7 +7225,7 @@
         <v>#DIV/0!</v>
       </c>
       <c r="U83" s="15"/>
-      <c r="V83" s="19"/>
+      <c r="V83" s="22"/>
       <c r="W83" s="4" t="s">
         <v>9</v>
       </c>
@@ -6528,14 +7238,24 @@
         <f t="shared" si="45"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="AD83" s="12"/>
-      <c r="AE83" s="13"/>
-      <c r="AF83" s="13"/>
-      <c r="AG83" s="13"/>
-      <c r="AH83" s="14"/>
-      <c r="AI83" s="5" t="e">
+      <c r="AD83" s="12">
+        <v>3064</v>
+      </c>
+      <c r="AE83" s="13">
+        <v>3279</v>
+      </c>
+      <c r="AF83" s="13">
+        <v>3105</v>
+      </c>
+      <c r="AG83" s="13">
+        <v>3277</v>
+      </c>
+      <c r="AH83" s="14">
+        <v>3127</v>
+      </c>
+      <c r="AI83" s="5">
         <f t="shared" si="46"/>
-        <v>#DIV/0!</v>
+        <v>3170.4</v>
       </c>
       <c r="AJ83" s="12"/>
       <c r="AK83" s="13"/>
@@ -6549,30 +7269,30 @@
     </row>
   </sheetData>
   <mergeCells count="24">
+    <mergeCell ref="A1:C2"/>
+    <mergeCell ref="A5:A13"/>
+    <mergeCell ref="C3:H3"/>
+    <mergeCell ref="I3:N3"/>
+    <mergeCell ref="A25:A33"/>
+    <mergeCell ref="AD3:AI3"/>
+    <mergeCell ref="AJ3:AO3"/>
+    <mergeCell ref="O3:T3"/>
+    <mergeCell ref="A15:A23"/>
+    <mergeCell ref="A75:A83"/>
+    <mergeCell ref="A35:A43"/>
+    <mergeCell ref="A45:A53"/>
+    <mergeCell ref="A55:A63"/>
+    <mergeCell ref="A65:A73"/>
+    <mergeCell ref="V35:V43"/>
+    <mergeCell ref="V45:V53"/>
+    <mergeCell ref="V55:V63"/>
+    <mergeCell ref="V65:V73"/>
+    <mergeCell ref="V75:V83"/>
     <mergeCell ref="V1:X2"/>
     <mergeCell ref="X3:AC3"/>
     <mergeCell ref="V5:V13"/>
     <mergeCell ref="V15:V23"/>
     <mergeCell ref="V25:V33"/>
-    <mergeCell ref="V35:V43"/>
-    <mergeCell ref="V45:V53"/>
-    <mergeCell ref="V55:V63"/>
-    <mergeCell ref="V65:V73"/>
-    <mergeCell ref="V75:V83"/>
-    <mergeCell ref="AD3:AI3"/>
-    <mergeCell ref="AJ3:AO3"/>
-    <mergeCell ref="O3:T3"/>
-    <mergeCell ref="A15:A23"/>
-    <mergeCell ref="A75:A83"/>
-    <mergeCell ref="A1:C2"/>
-    <mergeCell ref="A5:A13"/>
-    <mergeCell ref="C3:H3"/>
-    <mergeCell ref="I3:N3"/>
-    <mergeCell ref="A25:A33"/>
-    <mergeCell ref="A35:A43"/>
-    <mergeCell ref="A45:A53"/>
-    <mergeCell ref="A55:A63"/>
-    <mergeCell ref="A65:A73"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>